<commit_message>
modified fastq test data;
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D648B5-9D31-4E67-8021-57CDE4B8A63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97E495C-9B76-574E-BAE4-85572A0E12B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="825" windowWidth="20145" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="820" windowWidth="20140" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPXV_Metadata" sheetId="1" r:id="rId1"/>
@@ -1385,7 +1385,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2094,34 +2094,34 @@
   </sheetPr>
   <dimension ref="A1:BA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="23.42578125" customWidth="1"/>
-    <col min="15" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.42578125" customWidth="1"/>
-    <col min="40" max="49" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="16" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5" customWidth="1"/>
+    <col min="40" max="49" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="13.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="18.75" customHeight="1">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="18.75" customHeight="1">
+    <row r="2" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>423</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="18.75" customHeight="1">
+    <row r="3" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>429</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="18.75" customHeight="1">
+    <row r="4" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>430</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:53" ht="18.75" customHeight="1">
+    <row r="5" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>431</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="18.75" customHeight="1">
+    <row r="6" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>432</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="7" spans="1:53" ht="18.75" customHeight="1">
+    <row r="7" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>433</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="18.75" customHeight="1">
+    <row r="8" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y8" s="36"/>
       <c r="AE8" s="14"/>
       <c r="AP8" s="36"/>
@@ -2731,12 +2731,12 @@
       <c r="AY8" s="14"/>
       <c r="AZ8" s="14"/>
     </row>
-    <row r="9" spans="1:53" ht="18.75" customHeight="1">
+    <row r="9" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y9" s="36"/>
       <c r="AE9" s="14"/>
       <c r="AP9" s="36"/>
     </row>
-    <row r="10" spans="1:53" ht="18.75" customHeight="1">
+    <row r="10" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L10" s="36"/>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
@@ -2746,7 +2746,7 @@
       <c r="AG10" s="36"/>
       <c r="AP10" s="36"/>
     </row>
-    <row r="11" spans="1:53" ht="18.75" customHeight="1">
+    <row r="11" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L11" s="36"/>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
@@ -2756,7 +2756,7 @@
       <c r="AG11" s="36"/>
       <c r="AP11" s="36"/>
     </row>
-    <row r="12" spans="1:53" ht="18.75" customHeight="1">
+    <row r="12" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L12" s="36"/>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
@@ -2766,7 +2766,7 @@
       <c r="AG12" s="36"/>
       <c r="AP12" s="36"/>
     </row>
-    <row r="13" spans="1:53" ht="18.75" customHeight="1">
+    <row r="13" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L13" s="36"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
@@ -2776,7 +2776,7 @@
       <c r="AG13" s="36"/>
       <c r="AP13" s="36"/>
     </row>
-    <row r="14" spans="1:53" ht="18.75" customHeight="1">
+    <row r="14" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L14" s="36"/>
       <c r="M14" s="48"/>
       <c r="N14" s="48"/>
@@ -2786,7 +2786,7 @@
       <c r="AG14" s="36"/>
       <c r="AP14" s="36"/>
     </row>
-    <row r="15" spans="1:53" ht="18.75" customHeight="1">
+    <row r="15" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L15" s="36"/>
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
@@ -2796,7 +2796,7 @@
       <c r="AG15" s="36"/>
       <c r="AP15" s="36"/>
     </row>
-    <row r="16" spans="1:53" ht="18.75" customHeight="1">
+    <row r="16" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L16" s="36"/>
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
@@ -2806,7 +2806,7 @@
       <c r="AG16" s="36"/>
       <c r="AP16" s="36"/>
     </row>
-    <row r="17" spans="12:42" ht="18.75" customHeight="1">
+    <row r="17" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L17" s="36"/>
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
@@ -2816,7 +2816,7 @@
       <c r="AG17" s="36"/>
       <c r="AP17" s="36"/>
     </row>
-    <row r="18" spans="12:42" ht="18.75" customHeight="1">
+    <row r="18" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L18" s="36"/>
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
@@ -2826,7 +2826,7 @@
       <c r="AG18" s="36"/>
       <c r="AP18" s="36"/>
     </row>
-    <row r="19" spans="12:42" ht="18.75" customHeight="1">
+    <row r="19" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L19" s="36"/>
       <c r="M19" s="48"/>
       <c r="N19" s="48"/>
@@ -2836,7 +2836,7 @@
       <c r="AG19" s="36"/>
       <c r="AP19" s="36"/>
     </row>
-    <row r="20" spans="12:42" ht="18.75" customHeight="1">
+    <row r="20" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L20" s="36"/>
       <c r="M20" s="48"/>
       <c r="N20" s="48"/>
@@ -2846,7 +2846,7 @@
       <c r="AG20" s="36"/>
       <c r="AP20" s="36"/>
     </row>
-    <row r="21" spans="12:42" ht="18.75" customHeight="1">
+    <row r="21" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L21" s="36"/>
       <c r="M21" s="48"/>
       <c r="N21" s="48"/>
@@ -2856,7 +2856,7 @@
       <c r="AG21" s="36"/>
       <c r="AP21" s="36"/>
     </row>
-    <row r="22" spans="12:42" ht="18.75" customHeight="1">
+    <row r="22" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L22" s="36"/>
       <c r="M22" s="48"/>
       <c r="N22" s="48"/>
@@ -2866,7 +2866,7 @@
       <c r="AG22" s="36"/>
       <c r="AP22" s="36"/>
     </row>
-    <row r="23" spans="12:42" ht="18.75" customHeight="1">
+    <row r="23" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L23" s="36"/>
       <c r="M23" s="48"/>
       <c r="N23" s="48"/>
@@ -2876,7 +2876,7 @@
       <c r="AG23" s="36"/>
       <c r="AP23" s="36"/>
     </row>
-    <row r="24" spans="12:42" ht="18.75" customHeight="1">
+    <row r="24" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L24" s="36"/>
       <c r="M24" s="48"/>
       <c r="N24" s="48"/>
@@ -2886,7 +2886,7 @@
       <c r="AG24" s="36"/>
       <c r="AP24" s="36"/>
     </row>
-    <row r="25" spans="12:42" ht="18.75" customHeight="1">
+    <row r="25" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L25" s="36"/>
       <c r="M25" s="48"/>
       <c r="N25" s="48"/>
@@ -2896,7 +2896,7 @@
       <c r="AG25" s="36"/>
       <c r="AP25" s="36"/>
     </row>
-    <row r="26" spans="12:42" ht="18.75" customHeight="1">
+    <row r="26" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L26" s="36"/>
       <c r="M26" s="48"/>
       <c r="N26" s="48"/>
@@ -2906,7 +2906,7 @@
       <c r="AG26" s="36"/>
       <c r="AP26" s="36"/>
     </row>
-    <row r="27" spans="12:42" ht="18.75" customHeight="1">
+    <row r="27" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L27" s="36"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
@@ -2916,7 +2916,7 @@
       <c r="AG27" s="36"/>
       <c r="AP27" s="36"/>
     </row>
-    <row r="28" spans="12:42" ht="18.75" customHeight="1">
+    <row r="28" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L28" s="36"/>
       <c r="M28" s="48"/>
       <c r="N28" s="48"/>
@@ -2926,7 +2926,7 @@
       <c r="AG28" s="36"/>
       <c r="AP28" s="36"/>
     </row>
-    <row r="29" spans="12:42" ht="18.75" customHeight="1">
+    <row r="29" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L29" s="36"/>
       <c r="M29" s="48"/>
       <c r="N29" s="48"/>
@@ -2936,7 +2936,7 @@
       <c r="AG29" s="36"/>
       <c r="AP29" s="36"/>
     </row>
-    <row r="30" spans="12:42" ht="18.75" customHeight="1">
+    <row r="30" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L30" s="36"/>
       <c r="M30" s="48"/>
       <c r="N30" s="48"/>
@@ -2946,7 +2946,7 @@
       <c r="AG30" s="36"/>
       <c r="AP30" s="36"/>
     </row>
-    <row r="31" spans="12:42" ht="18.75" customHeight="1">
+    <row r="31" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L31" s="36"/>
       <c r="M31" s="48"/>
       <c r="N31" s="48"/>
@@ -2956,7 +2956,7 @@
       <c r="AG31" s="36"/>
       <c r="AP31" s="36"/>
     </row>
-    <row r="32" spans="12:42" ht="18.75" customHeight="1">
+    <row r="32" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L32" s="36"/>
       <c r="M32" s="48"/>
       <c r="N32" s="48"/>
@@ -2966,7 +2966,7 @@
       <c r="AG32" s="36"/>
       <c r="AP32" s="36"/>
     </row>
-    <row r="33" spans="12:42" ht="18.75" customHeight="1">
+    <row r="33" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L33" s="36"/>
       <c r="M33" s="48"/>
       <c r="N33" s="48"/>
@@ -2976,7 +2976,7 @@
       <c r="AG33" s="36"/>
       <c r="AP33" s="36"/>
     </row>
-    <row r="34" spans="12:42" ht="18.75" customHeight="1">
+    <row r="34" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L34" s="36"/>
       <c r="M34" s="48"/>
       <c r="N34" s="48"/>
@@ -2986,7 +2986,7 @@
       <c r="AG34" s="36"/>
       <c r="AP34" s="36"/>
     </row>
-    <row r="35" spans="12:42" ht="18.75" customHeight="1">
+    <row r="35" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L35" s="36"/>
       <c r="M35" s="48"/>
       <c r="N35" s="48"/>
@@ -2996,7 +2996,7 @@
       <c r="AG35" s="36"/>
       <c r="AP35" s="36"/>
     </row>
-    <row r="36" spans="12:42" ht="18.75" customHeight="1">
+    <row r="36" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L36" s="36"/>
       <c r="M36" s="48"/>
       <c r="N36" s="48"/>
@@ -3006,7 +3006,7 @@
       <c r="AG36" s="36"/>
       <c r="AP36" s="36"/>
     </row>
-    <row r="37" spans="12:42" ht="18.75" customHeight="1">
+    <row r="37" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L37" s="36"/>
       <c r="M37" s="48"/>
       <c r="N37" s="48"/>
@@ -3016,7 +3016,7 @@
       <c r="AG37" s="36"/>
       <c r="AP37" s="36"/>
     </row>
-    <row r="38" spans="12:42" ht="18.75" customHeight="1">
+    <row r="38" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L38" s="36"/>
       <c r="M38" s="48"/>
       <c r="N38" s="48"/>
@@ -3026,7 +3026,7 @@
       <c r="AG38" s="36"/>
       <c r="AP38" s="36"/>
     </row>
-    <row r="39" spans="12:42" ht="18.75" customHeight="1">
+    <row r="39" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L39" s="36"/>
       <c r="M39" s="48"/>
       <c r="N39" s="48"/>
@@ -3036,7 +3036,7 @@
       <c r="AG39" s="36"/>
       <c r="AP39" s="36"/>
     </row>
-    <row r="40" spans="12:42" ht="18.75" customHeight="1">
+    <row r="40" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L40" s="36"/>
       <c r="M40" s="48"/>
       <c r="N40" s="48"/>
@@ -3046,7 +3046,7 @@
       <c r="AG40" s="36"/>
       <c r="AP40" s="36"/>
     </row>
-    <row r="41" spans="12:42" ht="18.75" customHeight="1">
+    <row r="41" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L41" s="36"/>
       <c r="M41" s="48"/>
       <c r="N41" s="48"/>
@@ -3056,7 +3056,7 @@
       <c r="AG41" s="36"/>
       <c r="AP41" s="36"/>
     </row>
-    <row r="42" spans="12:42" ht="18.75" customHeight="1">
+    <row r="42" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L42" s="36"/>
       <c r="M42" s="48"/>
       <c r="N42" s="48"/>
@@ -3066,7 +3066,7 @@
       <c r="AG42" s="36"/>
       <c r="AP42" s="36"/>
     </row>
-    <row r="43" spans="12:42" ht="18.75" customHeight="1">
+    <row r="43" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L43" s="36"/>
       <c r="M43" s="48"/>
       <c r="N43" s="48"/>
@@ -3076,7 +3076,7 @@
       <c r="AG43" s="36"/>
       <c r="AP43" s="36"/>
     </row>
-    <row r="44" spans="12:42" ht="18.75" customHeight="1">
+    <row r="44" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L44" s="36"/>
       <c r="M44" s="48"/>
       <c r="N44" s="48"/>
@@ -3086,7 +3086,7 @@
       <c r="AG44" s="36"/>
       <c r="AP44" s="36"/>
     </row>
-    <row r="45" spans="12:42" ht="18.75" customHeight="1">
+    <row r="45" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L45" s="36"/>
       <c r="M45" s="48"/>
       <c r="N45" s="48"/>
@@ -3096,7 +3096,7 @@
       <c r="AG45" s="36"/>
       <c r="AP45" s="36"/>
     </row>
-    <row r="46" spans="12:42" ht="18.75" customHeight="1">
+    <row r="46" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L46" s="36"/>
       <c r="M46" s="48"/>
       <c r="N46" s="48"/>
@@ -3122,27 +3122,27 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="35" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="35" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18.75" customHeight="1">
+    <row r="2" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>222</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="18.75" customHeight="1">
+    <row r="3" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="18.75" customHeight="1">
+    <row r="4" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>339</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="18.75" customHeight="1">
+    <row r="5" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="36"/>
       <c r="M5" s="36"/>
       <c r="Q5" s="36"/>
@@ -3479,7 +3479,7 @@
       <c r="U5" s="36"/>
       <c r="AC5" s="36"/>
     </row>
-    <row r="6" spans="1:35" ht="18.75" customHeight="1">
+    <row r="6" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="36"/>
       <c r="M6" s="36"/>
       <c r="Q6" s="36"/>
@@ -3487,7 +3487,7 @@
       <c r="U6" s="36"/>
       <c r="AC6" s="36"/>
     </row>
-    <row r="7" spans="1:35" ht="18.75" customHeight="1">
+    <row r="7" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="36"/>
       <c r="M7" s="36"/>
       <c r="Q7" s="36"/>
@@ -3495,7 +3495,7 @@
       <c r="U7" s="36"/>
       <c r="AC7" s="36"/>
     </row>
-    <row r="8" spans="1:35" ht="18.75" customHeight="1">
+    <row r="8" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
         <v>341</v>
       </c>
@@ -3508,7 +3508,7 @@
       <c r="U8" s="36"/>
       <c r="AC8" s="36"/>
     </row>
-    <row r="9" spans="1:35" ht="18.75" customHeight="1">
+    <row r="9" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>317</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="18.75" customHeight="1">
+    <row r="10" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>222</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="18.75" customHeight="1">
+    <row r="11" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="U11" s="36"/>
       <c r="AC11" s="36"/>
     </row>
-    <row r="12" spans="1:35" ht="18.75" customHeight="1">
+    <row r="12" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>342</v>
       </c>
@@ -3728,7 +3728,7 @@
       <c r="U12" s="36"/>
       <c r="AC12" s="36"/>
     </row>
-    <row r="13" spans="1:35" ht="18.75" customHeight="1">
+    <row r="13" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="36"/>
       <c r="M13" s="36"/>
       <c r="Q13" s="36"/>
@@ -3736,7 +3736,7 @@
       <c r="U13" s="36"/>
       <c r="AC13" s="36"/>
     </row>
-    <row r="14" spans="1:35" ht="18.75" customHeight="1">
+    <row r="14" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
         <v>347</v>
       </c>
@@ -3749,7 +3749,7 @@
       <c r="U14" s="36"/>
       <c r="AC14" s="36"/>
     </row>
-    <row r="15" spans="1:35" ht="18.75" customHeight="1">
+    <row r="15" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>317</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="18.75" customHeight="1">
+    <row r="16" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>222</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="18.75" customHeight="1">
+    <row r="17" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>348</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="18.75" customHeight="1">
+    <row r="18" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>357</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="AC18" s="36"/>
     </row>
-    <row r="19" spans="1:35" ht="18.75" customHeight="1">
+    <row r="19" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>362</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="18.75" customHeight="1">
+    <row r="20" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="36"/>
       <c r="M20" s="36"/>
       <c r="Q20" s="36"/>
@@ -4078,7 +4078,7 @@
       <c r="U20" s="36"/>
       <c r="AC20" s="36"/>
     </row>
-    <row r="21" spans="1:35" ht="18.75" customHeight="1">
+    <row r="21" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="36"/>
       <c r="M21" s="36"/>
       <c r="Q21" s="36"/>
@@ -4086,7 +4086,7 @@
       <c r="U21" s="36"/>
       <c r="AC21" s="36"/>
     </row>
-    <row r="22" spans="1:35" ht="18.75" customHeight="1">
+    <row r="22" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="36"/>
       <c r="M22" s="36"/>
       <c r="Q22" s="36"/>
@@ -4094,7 +4094,7 @@
       <c r="U22" s="36"/>
       <c r="AC22" s="36"/>
     </row>
-    <row r="23" spans="1:35" ht="18.75" customHeight="1">
+    <row r="23" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -4111,7 +4111,7 @@
       <c r="U23" s="36"/>
       <c r="AC23" s="36"/>
     </row>
-    <row r="24" spans="1:35" ht="18.75" customHeight="1">
+    <row r="24" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="44" t="s">
         <v>367</v>
@@ -4130,7 +4130,7 @@
       <c r="U24" s="36"/>
       <c r="AC24" s="36"/>
     </row>
-    <row r="25" spans="1:35" ht="18.75" customHeight="1">
+    <row r="25" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
@@ -4147,7 +4147,7 @@
       <c r="U25" s="36"/>
       <c r="AC25" s="36"/>
     </row>
-    <row r="26" spans="1:35" ht="18.75" customHeight="1">
+    <row r="26" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -4164,7 +4164,7 @@
       <c r="U26" s="36"/>
       <c r="AC26" s="36"/>
     </row>
-    <row r="27" spans="1:35" ht="18.75" customHeight="1">
+    <row r="27" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -4181,7 +4181,7 @@
       <c r="U27" s="36"/>
       <c r="AC27" s="36"/>
     </row>
-    <row r="28" spans="1:35" ht="18.75" customHeight="1">
+    <row r="28" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="36"/>
       <c r="M28" s="36"/>
       <c r="Q28" s="36"/>
@@ -4189,7 +4189,7 @@
       <c r="U28" s="36"/>
       <c r="AC28" s="36"/>
     </row>
-    <row r="29" spans="1:35" ht="18.75" customHeight="1">
+    <row r="29" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="36"/>
       <c r="M29" s="36"/>
       <c r="Q29" s="36"/>
@@ -4197,7 +4197,7 @@
       <c r="U29" s="36"/>
       <c r="AC29" s="36"/>
     </row>
-    <row r="30" spans="1:35" ht="18.75" customHeight="1">
+    <row r="30" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="36"/>
       <c r="M30" s="36"/>
       <c r="Q30" s="36"/>
@@ -4219,30 +4219,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75" customHeight="1">
+    <row r="1" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>222</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="18.75" customHeight="1">
+    <row r="2" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>301</v>
       </c>
@@ -4497,24 +4497,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18.75" customHeight="1">
+    <row r="3" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>278</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="18.75" customHeight="1">
+    <row r="4" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O4" s="19"/>
     </row>
   </sheetData>
@@ -4709,20 +4709,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>253</v>
       </c>
@@ -4926,22 +4926,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -4954,7 +4954,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4988,7 +4988,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -5022,7 +5022,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -5039,7 +5039,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -5056,7 +5056,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -5073,7 +5073,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -5090,7 +5090,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -5107,7 +5107,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -5141,7 +5141,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -5175,7 +5175,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -5192,7 +5192,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -5209,7 +5209,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="18.75" customHeight="1">
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -5226,7 +5226,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -5243,7 +5243,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -5260,7 +5260,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1">
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -5277,7 +5277,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -5294,7 +5294,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -5328,7 +5328,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1">
+    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -5345,7 +5345,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1">
+    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -5377,7 +5377,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1">
+    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -5394,7 +5394,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -5411,7 +5411,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -5428,7 +5428,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -5445,7 +5445,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="18.75" customHeight="1">
+    <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -5460,7 +5460,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="18.75" customHeight="1">
+    <row r="32" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -5477,7 +5477,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="18.75" customHeight="1">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -5494,7 +5494,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="18.75" customHeight="1">
+    <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -5511,7 +5511,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="18.75" customHeight="1">
+    <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
@@ -5526,7 +5526,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="18.75" customHeight="1">
+    <row r="36" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -5541,7 +5541,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="18.75" customHeight="1">
+    <row r="37" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -5558,7 +5558,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="18.75" customHeight="1">
+    <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="50"/>
       <c r="C38" s="50"/>
@@ -5571,7 +5571,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="18.75" customHeight="1">
+    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
@@ -5588,7 +5588,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="18.75" customHeight="1">
+    <row r="40" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
@@ -5605,7 +5605,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="18.75" customHeight="1">
+    <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
@@ -5622,7 +5622,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="18.75" customHeight="1">
+    <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
@@ -5639,7 +5639,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="18.75" customHeight="1">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
@@ -5656,7 +5656,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="18.75" customHeight="1">
+    <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
@@ -5673,7 +5673,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="18.75" customHeight="1">
+    <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
@@ -5690,7 +5690,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="18.75" customHeight="1">
+    <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -5705,7 +5705,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="18.75" customHeight="1">
+    <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -5720,7 +5720,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="18.75" customHeight="1">
+    <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -5737,7 +5737,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="18.75" customHeight="1">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="50"/>
       <c r="C49" s="50"/>
@@ -5750,7 +5750,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="18.75" customHeight="1">
+    <row r="50" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -5767,7 +5767,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="18.75" customHeight="1">
+    <row r="51" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="18.75" customHeight="1">
+    <row r="52" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
@@ -5801,7 +5801,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="18.75" customHeight="1">
+    <row r="53" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="18.75" customHeight="1">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
@@ -5835,7 +5835,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="18.75" customHeight="1">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
@@ -5852,7 +5852,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="18.75" customHeight="1">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
@@ -5869,7 +5869,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="18.75" customHeight="1">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -5886,7 +5886,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="18.75" customHeight="1">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -5903,7 +5903,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="18.75" customHeight="1">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
@@ -5920,7 +5920,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="18.75" customHeight="1">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
@@ -5937,7 +5937,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="18.75" customHeight="1">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
@@ -5954,7 +5954,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" ht="18.75" customHeight="1">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -5971,7 +5971,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="18.75" customHeight="1">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
@@ -5988,7 +5988,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="18.75" customHeight="1">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
@@ -6005,7 +6005,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" ht="18.75" customHeight="1">
+    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
@@ -6022,7 +6022,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="18.75" customHeight="1">
+    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" ht="18.75" customHeight="1">
+    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -6056,7 +6056,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="18.75" customHeight="1">
+    <row r="68" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
@@ -6073,7 +6073,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" ht="18.75" customHeight="1">
+    <row r="69" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" ht="18.75" customHeight="1">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
@@ -6107,7 +6107,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" ht="18.75" customHeight="1">
+    <row r="71" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
@@ -6124,7 +6124,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="18.75" customHeight="1">
+    <row r="72" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
@@ -6141,7 +6141,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" ht="18.75" customHeight="1">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
@@ -6158,7 +6158,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" ht="18.75" customHeight="1">
+    <row r="74" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
@@ -6175,7 +6175,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" ht="18.75" customHeight="1">
+    <row r="75" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
@@ -6192,7 +6192,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" ht="18.75" customHeight="1">
+    <row r="76" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" ht="18.75" customHeight="1">
+    <row r="77" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
@@ -6226,7 +6226,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" ht="18.75" customHeight="1">
+    <row r="78" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>139</v>
       </c>
@@ -6241,7 +6241,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="18.75" customHeight="1">
+    <row r="79" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
@@ -6256,7 +6256,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="18.75" customHeight="1">
+    <row r="80" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>141</v>
       </c>
@@ -6273,7 +6273,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" ht="18.75" customHeight="1">
+    <row r="81" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
@@ -6290,7 +6290,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" ht="18.75" customHeight="1">
+    <row r="82" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>145</v>
       </c>
@@ -6307,7 +6307,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="18.75" customHeight="1">
+    <row r="83" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>147</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" ht="18.75" customHeight="1">
+    <row r="84" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="2"/>
@@ -6337,7 +6337,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" ht="18.75" customHeight="1">
+    <row r="85" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>149</v>
       </c>
@@ -6352,7 +6352,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" ht="18.75" customHeight="1">
+    <row r="86" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>150</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="18.75" customHeight="1">
+    <row r="87" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>153</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="18.75" customHeight="1">
+    <row r="88" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>159</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="18.75" customHeight="1">
+    <row r="89" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>157</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18.75" customHeight="1">
+    <row r="90" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>154</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18.75" customHeight="1">
+    <row r="91" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>152</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="18.75" customHeight="1">
+    <row r="92" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>151</v>
       </c>
@@ -6561,7 +6561,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="18.75" customHeight="1">
+    <row r="93" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -6582,7 +6582,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="18.75" customHeight="1">
+    <row r="94" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>158</v>
       </c>
@@ -6601,7 +6601,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" ht="18.75" customHeight="1">
+    <row r="95" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>155</v>
       </c>
@@ -6620,7 +6620,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" ht="18.75" customHeight="1">
+    <row r="96" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
@@ -6637,7 +6637,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" ht="18.75" customHeight="1">
+    <row r="97" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
@@ -6652,7 +6652,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" ht="18.75" customHeight="1">
+    <row r="98" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
@@ -6667,7 +6667,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" ht="18.75" customHeight="1">
+    <row r="99" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
@@ -6682,7 +6682,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" ht="18.75" customHeight="1">
+    <row r="100" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="C100" s="8" t="s">
@@ -6697,7 +6697,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" ht="18.75" customHeight="1">
+    <row r="101" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="7" t="s">
@@ -6712,7 +6712,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" ht="18.75" customHeight="1">
+    <row r="102" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
@@ -6727,7 +6727,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" ht="18.75" customHeight="1">
+    <row r="103" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
@@ -6742,7 +6742,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" ht="18.75" customHeight="1">
+    <row r="104" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
@@ -6757,7 +6757,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" ht="18.75" customHeight="1">
+    <row r="105" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1" t="s">
@@ -6772,7 +6772,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" ht="18.75" customHeight="1">
+    <row r="106" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1" t="s">
@@ -6787,7 +6787,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" ht="18.75" customHeight="1">
+    <row r="107" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1" t="s">
@@ -6804,6 +6804,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6812,61 +6867,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove fasta_file_name from example metadata file
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97E495C-9B76-574E-BAE4-85572A0E12B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA88695A-937D-4718-8E6C-889B728FCFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="820" windowWidth="20140" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPXV_Metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="441">
   <si>
     <t>Strategy</t>
   </si>
@@ -1325,21 +1325,6 @@
   </si>
   <si>
     <t>TX0001_7.fasta</t>
-  </si>
-  <si>
-    <t>FL0004.fasta</t>
-  </si>
-  <si>
-    <t>IL0005.fasta</t>
-  </si>
-  <si>
-    <t>NY0006.fasta</t>
-  </si>
-  <si>
-    <t>NY0007.fasta</t>
-  </si>
-  <si>
-    <t>TX0001.fasta</t>
   </si>
   <si>
     <t>ncbi-spuid</t>
@@ -1385,7 +1370,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1470,7 +1455,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1530,12 +1515,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1640,7 +1619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1771,7 +1750,6 @@
     <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2092,1019 +2070,1001 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BA46"/>
+  <dimension ref="A1:AZ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="23.5" customWidth="1"/>
-    <col min="15" max="16" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="30" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5" customWidth="1"/>
-    <col min="40" max="49" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="37" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.42578125" customWidth="1"/>
+    <col min="39" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>317</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="Y1" s="36" t="s">
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="X1" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="AC1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>320</v>
       </c>
+      <c r="AE1" s="36" t="s">
+        <v>321</v>
+      </c>
       <c r="AF1" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="AG1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AP1" s="36" t="s">
+      <c r="AO1" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A2" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>431</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>432</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="U2" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="V2" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB2" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="AE2" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF2" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL2" s="46" t="s">
+        <v>433</v>
+      </c>
+      <c r="AM2" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="AO2" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="AP2" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="AQ2" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="AR2" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="AS2" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="AU2" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="AW2" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="AX2" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="AY2" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="AZ2" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>368</v>
-      </c>
-      <c r="C2" s="47" t="s">
+    </row>
+    <row r="3" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E3" t="s">
+        <v>380</v>
+      </c>
+      <c r="K3" t="s">
+        <v>379</v>
+      </c>
+      <c r="O3" t="s">
+        <v>257</v>
+      </c>
+      <c r="P3" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>350</v>
+      </c>
+      <c r="R3" t="s">
+        <v>307</v>
+      </c>
+      <c r="S3" t="s">
+        <v>262</v>
+      </c>
+      <c r="T3" t="s">
+        <v>382</v>
+      </c>
+      <c r="V3" t="s">
+        <v>383</v>
+      </c>
+      <c r="X3" s="36"/>
+      <c r="AB3" t="s">
+        <v>384</v>
+      </c>
+      <c r="AD3" s="14">
+        <v>247</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>385</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL3" t="s">
         <v>434</v>
       </c>
-      <c r="D2" s="47" t="s">
-        <v>435</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>436</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>369</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>441</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>442</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>443</v>
-      </c>
-      <c r="J2" s="49" t="s">
-        <v>444</v>
-      </c>
-      <c r="K2" s="49" t="s">
-        <v>445</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>370</v>
-      </c>
-      <c r="M2" s="49" t="s">
-        <v>440</v>
-      </c>
-      <c r="N2" s="49" t="s">
-        <v>437</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>373</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="U2" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="V2" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="W2" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y2" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="Z2" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="AA2" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB2" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC2" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="AD2" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="AF2" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="AG2" s="37" t="s">
-        <v>288</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="AJ2" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="AK2" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="AL2" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="AM2" s="47" t="s">
-        <v>438</v>
-      </c>
-      <c r="AN2" s="47" t="s">
-        <v>298</v>
-      </c>
-      <c r="AO2" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="AP2" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="AQ2" s="20" t="s">
-        <v>328</v>
-      </c>
-      <c r="AR2" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="AS2" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="AT2" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="AU2" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="AV2" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="AX2" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="AY2" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="AZ2" s="21" t="s">
-        <v>377</v>
-      </c>
-      <c r="BA2" s="45" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F3" t="s">
-        <v>380</v>
-      </c>
-      <c r="L3" t="s">
-        <v>379</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="AM3" t="s">
+        <v>386</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>387</v>
+      </c>
+      <c r="AO3" s="36"/>
+      <c r="AW3" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="AX3" s="17">
+        <v>50</v>
+      </c>
+      <c r="AY3" s="14">
+        <v>1</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E4" t="s">
+        <v>391</v>
+      </c>
+      <c r="K4" t="s">
+        <v>390</v>
+      </c>
+      <c r="O4" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="P4" t="s">
         <v>381</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q4" t="s">
         <v>350</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R4" t="s">
         <v>307</v>
       </c>
-      <c r="T3" t="s">
-        <v>262</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="S4" t="s">
+        <v>392</v>
+      </c>
+      <c r="V4" t="s">
+        <v>393</v>
+      </c>
+      <c r="X4" s="36"/>
+      <c r="AB4" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD4" s="14">
+        <v>40</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>395</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>434</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>397</v>
+      </c>
+      <c r="AO4" s="36"/>
+      <c r="AW4" s="14">
+        <v>5</v>
+      </c>
+      <c r="AX4" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="AY4" s="14">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E5" t="s">
+        <v>400</v>
+      </c>
+      <c r="K5" t="s">
+        <v>399</v>
+      </c>
+      <c r="O5" t="s">
+        <v>257</v>
+      </c>
+      <c r="P5" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>350</v>
+      </c>
+      <c r="R5" t="s">
+        <v>307</v>
+      </c>
+      <c r="S5" t="s">
+        <v>401</v>
+      </c>
+      <c r="V5" t="s">
+        <v>402</v>
+      </c>
+      <c r="X5" s="36"/>
+      <c r="AB5" t="s">
+        <v>403</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>121</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>404</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>434</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>405</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>406</v>
+      </c>
+      <c r="AO5" s="36"/>
+      <c r="AW5" s="14">
+        <v>8</v>
+      </c>
+      <c r="AX5" s="14">
+        <v>3</v>
+      </c>
+      <c r="AY5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E6" t="s">
+        <v>400</v>
+      </c>
+      <c r="K6" t="s">
+        <v>408</v>
+      </c>
+      <c r="O6" t="s">
+        <v>257</v>
+      </c>
+      <c r="P6" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>350</v>
+      </c>
+      <c r="R6" t="s">
+        <v>307</v>
+      </c>
+      <c r="S6" t="s">
+        <v>401</v>
+      </c>
+      <c r="T6" t="s">
         <v>382</v>
       </c>
-      <c r="W3" t="s">
+      <c r="V6" t="s">
+        <v>409</v>
+      </c>
+      <c r="X6" s="36"/>
+      <c r="AB6" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD6" s="14">
+        <v>72</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>411</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>434</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>412</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>413</v>
+      </c>
+      <c r="AO6" s="36"/>
+      <c r="AW6" s="14">
+        <v>4</v>
+      </c>
+      <c r="AX6" s="16">
+        <v>3.2</v>
+      </c>
+      <c r="AY6" s="14">
+        <v>1</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B7" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" t="s">
+        <v>416</v>
+      </c>
+      <c r="K7" t="s">
+        <v>415</v>
+      </c>
+      <c r="O7" t="s">
+        <v>257</v>
+      </c>
+      <c r="P7" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>350</v>
+      </c>
+      <c r="R7" t="s">
+        <v>307</v>
+      </c>
+      <c r="S7" t="s">
+        <v>417</v>
+      </c>
+      <c r="T7" t="s">
+        <v>382</v>
+      </c>
+      <c r="V7" t="s">
         <v>383</v>
       </c>
-      <c r="Y3" s="36"/>
-      <c r="AC3" t="s">
-        <v>384</v>
-      </c>
-      <c r="AE3" s="14">
-        <v>247</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>385</v>
-      </c>
-      <c r="AG3" t="s">
+      <c r="X7" s="36"/>
+      <c r="AB7" t="s">
+        <v>418</v>
+      </c>
+      <c r="AD7" s="14">
+        <v>73</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>419</v>
+      </c>
+      <c r="AF7" t="s">
         <v>216</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AG7" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AH7" t="s">
         <v>73</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AI7" t="s">
         <v>85</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AJ7" t="s">
         <v>310</v>
       </c>
-      <c r="AM3" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>386</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>387</v>
-      </c>
-      <c r="AP3" s="36"/>
-      <c r="AX3" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="AY3" s="17">
-        <v>50</v>
-      </c>
-      <c r="AZ3" s="14">
-        <v>1</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>430</v>
-      </c>
-      <c r="B4" t="s">
-        <v>389</v>
-      </c>
-      <c r="C4" t="s">
-        <v>390</v>
-      </c>
-      <c r="F4" t="s">
-        <v>391</v>
-      </c>
-      <c r="L4" t="s">
-        <v>390</v>
-      </c>
-      <c r="P4" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>381</v>
-      </c>
-      <c r="R4" t="s">
-        <v>350</v>
-      </c>
-      <c r="S4" t="s">
-        <v>307</v>
-      </c>
-      <c r="T4" t="s">
-        <v>392</v>
-      </c>
-      <c r="W4" t="s">
-        <v>393</v>
-      </c>
-      <c r="Y4" s="36"/>
-      <c r="AC4" t="s">
-        <v>394</v>
-      </c>
-      <c r="AE4" s="14">
-        <v>40</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>395</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>216</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>396</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>397</v>
-      </c>
-      <c r="AP4" s="36"/>
-      <c r="AX4" s="14">
-        <v>5</v>
-      </c>
-      <c r="AY4" s="16">
-        <v>3.5</v>
-      </c>
-      <c r="AZ4" s="14">
+      <c r="AL7" t="s">
+        <v>434</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>420</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>421</v>
+      </c>
+      <c r="AO7" s="36"/>
+      <c r="AW7" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="AX7" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="AY7" s="14">
         <v>0</v>
       </c>
-      <c r="BA4" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>431</v>
-      </c>
-      <c r="B5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C5" t="s">
-        <v>399</v>
-      </c>
-      <c r="F5" t="s">
-        <v>400</v>
-      </c>
-      <c r="L5" t="s">
-        <v>399</v>
-      </c>
-      <c r="P5" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>381</v>
-      </c>
-      <c r="R5" t="s">
-        <v>350</v>
-      </c>
-      <c r="S5" t="s">
-        <v>307</v>
-      </c>
-      <c r="T5" t="s">
-        <v>401</v>
-      </c>
-      <c r="W5" t="s">
-        <v>402</v>
-      </c>
-      <c r="Y5" s="36"/>
-      <c r="AC5" t="s">
-        <v>403</v>
-      </c>
-      <c r="AE5" s="14">
-        <v>121</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>404</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>216</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>405</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>406</v>
-      </c>
-      <c r="AP5" s="36"/>
-      <c r="AX5" s="14">
-        <v>8</v>
-      </c>
-      <c r="AY5" s="14">
-        <v>3</v>
-      </c>
-      <c r="AZ5" s="14">
-        <v>0</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>432</v>
-      </c>
-      <c r="B6" t="s">
-        <v>407</v>
-      </c>
-      <c r="C6" t="s">
-        <v>408</v>
-      </c>
-      <c r="F6" t="s">
-        <v>400</v>
-      </c>
-      <c r="L6" t="s">
-        <v>408</v>
-      </c>
-      <c r="P6" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>381</v>
-      </c>
-      <c r="R6" t="s">
-        <v>350</v>
-      </c>
-      <c r="S6" t="s">
-        <v>307</v>
-      </c>
-      <c r="T6" t="s">
-        <v>401</v>
-      </c>
-      <c r="U6" t="s">
-        <v>382</v>
-      </c>
-      <c r="W6" t="s">
-        <v>409</v>
-      </c>
-      <c r="Y6" s="36"/>
-      <c r="AC6" t="s">
-        <v>410</v>
-      </c>
-      <c r="AE6" s="14">
-        <v>72</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>411</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>412</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>413</v>
-      </c>
-      <c r="AP6" s="36"/>
-      <c r="AX6" s="14">
-        <v>4</v>
-      </c>
-      <c r="AY6" s="16">
-        <v>3.2</v>
-      </c>
-      <c r="AZ6" s="14">
-        <v>1</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>433</v>
-      </c>
-      <c r="B7" t="s">
-        <v>414</v>
-      </c>
-      <c r="C7" t="s">
-        <v>415</v>
-      </c>
-      <c r="F7" t="s">
-        <v>416</v>
-      </c>
-      <c r="L7" t="s">
-        <v>415</v>
-      </c>
-      <c r="P7" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>381</v>
-      </c>
-      <c r="R7" t="s">
-        <v>350</v>
-      </c>
-      <c r="S7" t="s">
-        <v>307</v>
-      </c>
-      <c r="T7" t="s">
-        <v>417</v>
-      </c>
-      <c r="U7" t="s">
-        <v>382</v>
-      </c>
-      <c r="W7" t="s">
-        <v>383</v>
-      </c>
-      <c r="Y7" s="36"/>
-      <c r="AC7" t="s">
-        <v>418</v>
-      </c>
-      <c r="AE7" s="14">
-        <v>73</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>419</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>420</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>421</v>
-      </c>
-      <c r="AP7" s="36"/>
-      <c r="AX7" s="17" t="s">
-        <v>422</v>
-      </c>
-      <c r="AY7" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="AZ7" s="14">
-        <v>0</v>
-      </c>
-      <c r="BA7" t="s">
+      <c r="AZ7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y8" s="36"/>
-      <c r="AE8" s="14"/>
-      <c r="AP8" s="36"/>
+    <row r="8" spans="1:52" ht="18.75" customHeight="1">
+      <c r="X8" s="36"/>
+      <c r="AD8" s="14"/>
+      <c r="AO8" s="36"/>
+      <c r="AW8" s="14"/>
       <c r="AX8" s="14"/>
       <c r="AY8" s="14"/>
-      <c r="AZ8" s="14"/>
-    </row>
-    <row r="9" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y9" s="36"/>
-      <c r="AE9" s="14"/>
-      <c r="AP9" s="36"/>
-    </row>
-    <row r="10" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="36"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="Y10" s="36"/>
-      <c r="AC10" s="36"/>
+    </row>
+    <row r="9" spans="1:52" ht="18.75" customHeight="1">
+      <c r="X9" s="36"/>
+      <c r="AD9" s="14"/>
+      <c r="AO9" s="36"/>
+    </row>
+    <row r="10" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K10" s="36"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="X10" s="36"/>
+      <c r="AB10" s="36"/>
+      <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
-      <c r="AG10" s="36"/>
-      <c r="AP10" s="36"/>
-    </row>
-    <row r="11" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L11" s="36"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="Y11" s="36"/>
-      <c r="AC11" s="36"/>
+      <c r="AO10" s="36"/>
+    </row>
+    <row r="11" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K11" s="36"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="X11" s="36"/>
+      <c r="AB11" s="36"/>
+      <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
-      <c r="AG11" s="36"/>
-      <c r="AP11" s="36"/>
-    </row>
-    <row r="12" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L12" s="36"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="Y12" s="36"/>
-      <c r="AC12" s="36"/>
+      <c r="AO11" s="36"/>
+    </row>
+    <row r="12" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K12" s="36"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="X12" s="36"/>
+      <c r="AB12" s="36"/>
+      <c r="AE12" s="36"/>
       <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
-      <c r="AP12" s="36"/>
-    </row>
-    <row r="13" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L13" s="36"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="Y13" s="36"/>
-      <c r="AC13" s="36"/>
+      <c r="AO12" s="36"/>
+    </row>
+    <row r="13" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K13" s="36"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="X13" s="36"/>
+      <c r="AB13" s="36"/>
+      <c r="AE13" s="36"/>
       <c r="AF13" s="36"/>
-      <c r="AG13" s="36"/>
-      <c r="AP13" s="36"/>
-    </row>
-    <row r="14" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L14" s="36"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="Y14" s="36"/>
-      <c r="AC14" s="36"/>
+      <c r="AO13" s="36"/>
+    </row>
+    <row r="14" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K14" s="36"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="X14" s="36"/>
+      <c r="AB14" s="36"/>
+      <c r="AE14" s="36"/>
       <c r="AF14" s="36"/>
-      <c r="AG14" s="36"/>
-      <c r="AP14" s="36"/>
-    </row>
-    <row r="15" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L15" s="36"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="Y15" s="36"/>
-      <c r="AC15" s="36"/>
+      <c r="AO14" s="36"/>
+    </row>
+    <row r="15" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K15" s="36"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="X15" s="36"/>
+      <c r="AB15" s="36"/>
+      <c r="AE15" s="36"/>
       <c r="AF15" s="36"/>
-      <c r="AG15" s="36"/>
-      <c r="AP15" s="36"/>
-    </row>
-    <row r="16" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L16" s="36"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="Y16" s="36"/>
-      <c r="AC16" s="36"/>
+      <c r="AO15" s="36"/>
+    </row>
+    <row r="16" spans="1:52" ht="18.75" customHeight="1">
+      <c r="K16" s="36"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="X16" s="36"/>
+      <c r="AB16" s="36"/>
+      <c r="AE16" s="36"/>
       <c r="AF16" s="36"/>
-      <c r="AG16" s="36"/>
-      <c r="AP16" s="36"/>
-    </row>
-    <row r="17" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L17" s="36"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="Y17" s="36"/>
-      <c r="AC17" s="36"/>
+      <c r="AO16" s="36"/>
+    </row>
+    <row r="17" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K17" s="36"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="X17" s="36"/>
+      <c r="AB17" s="36"/>
+      <c r="AE17" s="36"/>
       <c r="AF17" s="36"/>
-      <c r="AG17" s="36"/>
-      <c r="AP17" s="36"/>
-    </row>
-    <row r="18" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L18" s="36"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="Y18" s="36"/>
-      <c r="AC18" s="36"/>
+      <c r="AO17" s="36"/>
+    </row>
+    <row r="18" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K18" s="36"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="X18" s="36"/>
+      <c r="AB18" s="36"/>
+      <c r="AE18" s="36"/>
       <c r="AF18" s="36"/>
-      <c r="AG18" s="36"/>
-      <c r="AP18" s="36"/>
-    </row>
-    <row r="19" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L19" s="36"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="Y19" s="36"/>
-      <c r="AC19" s="36"/>
+      <c r="AO18" s="36"/>
+    </row>
+    <row r="19" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K19" s="36"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="X19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AE19" s="36"/>
       <c r="AF19" s="36"/>
-      <c r="AG19" s="36"/>
-      <c r="AP19" s="36"/>
-    </row>
-    <row r="20" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L20" s="36"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="Y20" s="36"/>
-      <c r="AC20" s="36"/>
+      <c r="AO19" s="36"/>
+    </row>
+    <row r="20" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K20" s="36"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="X20" s="36"/>
+      <c r="AB20" s="36"/>
+      <c r="AE20" s="36"/>
       <c r="AF20" s="36"/>
-      <c r="AG20" s="36"/>
-      <c r="AP20" s="36"/>
-    </row>
-    <row r="21" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L21" s="36"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="Y21" s="36"/>
-      <c r="AC21" s="36"/>
+      <c r="AO20" s="36"/>
+    </row>
+    <row r="21" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K21" s="36"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="X21" s="36"/>
+      <c r="AB21" s="36"/>
+      <c r="AE21" s="36"/>
       <c r="AF21" s="36"/>
-      <c r="AG21" s="36"/>
-      <c r="AP21" s="36"/>
-    </row>
-    <row r="22" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L22" s="36"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="Y22" s="36"/>
-      <c r="AC22" s="36"/>
+      <c r="AO21" s="36"/>
+    </row>
+    <row r="22" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K22" s="36"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="X22" s="36"/>
+      <c r="AB22" s="36"/>
+      <c r="AE22" s="36"/>
       <c r="AF22" s="36"/>
-      <c r="AG22" s="36"/>
-      <c r="AP22" s="36"/>
-    </row>
-    <row r="23" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L23" s="36"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="Y23" s="36"/>
-      <c r="AC23" s="36"/>
+      <c r="AO22" s="36"/>
+    </row>
+    <row r="23" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K23" s="36"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="X23" s="36"/>
+      <c r="AB23" s="36"/>
+      <c r="AE23" s="36"/>
       <c r="AF23" s="36"/>
-      <c r="AG23" s="36"/>
-      <c r="AP23" s="36"/>
-    </row>
-    <row r="24" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L24" s="36"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="Y24" s="36"/>
-      <c r="AC24" s="36"/>
+      <c r="AO23" s="36"/>
+    </row>
+    <row r="24" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K24" s="36"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="X24" s="36"/>
+      <c r="AB24" s="36"/>
+      <c r="AE24" s="36"/>
       <c r="AF24" s="36"/>
-      <c r="AG24" s="36"/>
-      <c r="AP24" s="36"/>
-    </row>
-    <row r="25" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L25" s="36"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="Y25" s="36"/>
-      <c r="AC25" s="36"/>
+      <c r="AO24" s="36"/>
+    </row>
+    <row r="25" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K25" s="36"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="X25" s="36"/>
+      <c r="AB25" s="36"/>
+      <c r="AE25" s="36"/>
       <c r="AF25" s="36"/>
-      <c r="AG25" s="36"/>
-      <c r="AP25" s="36"/>
-    </row>
-    <row r="26" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L26" s="36"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="Y26" s="36"/>
-      <c r="AC26" s="36"/>
+      <c r="AO25" s="36"/>
+    </row>
+    <row r="26" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K26" s="36"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="X26" s="36"/>
+      <c r="AB26" s="36"/>
+      <c r="AE26" s="36"/>
       <c r="AF26" s="36"/>
-      <c r="AG26" s="36"/>
-      <c r="AP26" s="36"/>
-    </row>
-    <row r="27" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L27" s="36"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="Y27" s="36"/>
-      <c r="AC27" s="36"/>
+      <c r="AO26" s="36"/>
+    </row>
+    <row r="27" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K27" s="36"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="X27" s="36"/>
+      <c r="AB27" s="36"/>
+      <c r="AE27" s="36"/>
       <c r="AF27" s="36"/>
-      <c r="AG27" s="36"/>
-      <c r="AP27" s="36"/>
-    </row>
-    <row r="28" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L28" s="36"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="Y28" s="36"/>
-      <c r="AC28" s="36"/>
+      <c r="AO27" s="36"/>
+    </row>
+    <row r="28" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K28" s="36"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="X28" s="36"/>
+      <c r="AB28" s="36"/>
+      <c r="AE28" s="36"/>
       <c r="AF28" s="36"/>
-      <c r="AG28" s="36"/>
-      <c r="AP28" s="36"/>
-    </row>
-    <row r="29" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L29" s="36"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="Y29" s="36"/>
-      <c r="AC29" s="36"/>
+      <c r="AO28" s="36"/>
+    </row>
+    <row r="29" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K29" s="36"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="X29" s="36"/>
+      <c r="AB29" s="36"/>
+      <c r="AE29" s="36"/>
       <c r="AF29" s="36"/>
-      <c r="AG29" s="36"/>
-      <c r="AP29" s="36"/>
-    </row>
-    <row r="30" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L30" s="36"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="Y30" s="36"/>
-      <c r="AC30" s="36"/>
+      <c r="AO29" s="36"/>
+    </row>
+    <row r="30" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K30" s="36"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="X30" s="36"/>
+      <c r="AB30" s="36"/>
+      <c r="AE30" s="36"/>
       <c r="AF30" s="36"/>
-      <c r="AG30" s="36"/>
-      <c r="AP30" s="36"/>
-    </row>
-    <row r="31" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L31" s="36"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="Y31" s="36"/>
-      <c r="AC31" s="36"/>
+      <c r="AO30" s="36"/>
+    </row>
+    <row r="31" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K31" s="36"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="X31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AE31" s="36"/>
       <c r="AF31" s="36"/>
-      <c r="AG31" s="36"/>
-      <c r="AP31" s="36"/>
-    </row>
-    <row r="32" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L32" s="36"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="Y32" s="36"/>
-      <c r="AC32" s="36"/>
+      <c r="AO31" s="36"/>
+    </row>
+    <row r="32" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K32" s="36"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="X32" s="36"/>
+      <c r="AB32" s="36"/>
+      <c r="AE32" s="36"/>
       <c r="AF32" s="36"/>
-      <c r="AG32" s="36"/>
-      <c r="AP32" s="36"/>
-    </row>
-    <row r="33" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L33" s="36"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="Y33" s="36"/>
-      <c r="AC33" s="36"/>
+      <c r="AO32" s="36"/>
+    </row>
+    <row r="33" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K33" s="36"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="X33" s="36"/>
+      <c r="AB33" s="36"/>
+      <c r="AE33" s="36"/>
       <c r="AF33" s="36"/>
-      <c r="AG33" s="36"/>
-      <c r="AP33" s="36"/>
-    </row>
-    <row r="34" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L34" s="36"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="Y34" s="36"/>
-      <c r="AC34" s="36"/>
+      <c r="AO33" s="36"/>
+    </row>
+    <row r="34" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K34" s="36"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="X34" s="36"/>
+      <c r="AB34" s="36"/>
+      <c r="AE34" s="36"/>
       <c r="AF34" s="36"/>
-      <c r="AG34" s="36"/>
-      <c r="AP34" s="36"/>
-    </row>
-    <row r="35" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L35" s="36"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="Y35" s="36"/>
-      <c r="AC35" s="36"/>
+      <c r="AO34" s="36"/>
+    </row>
+    <row r="35" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K35" s="36"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="X35" s="36"/>
+      <c r="AB35" s="36"/>
+      <c r="AE35" s="36"/>
       <c r="AF35" s="36"/>
-      <c r="AG35" s="36"/>
-      <c r="AP35" s="36"/>
-    </row>
-    <row r="36" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L36" s="36"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="Y36" s="36"/>
-      <c r="AC36" s="36"/>
+      <c r="AO35" s="36"/>
+    </row>
+    <row r="36" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K36" s="36"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="X36" s="36"/>
+      <c r="AB36" s="36"/>
+      <c r="AE36" s="36"/>
       <c r="AF36" s="36"/>
-      <c r="AG36" s="36"/>
-      <c r="AP36" s="36"/>
-    </row>
-    <row r="37" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L37" s="36"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="Y37" s="36"/>
-      <c r="AC37" s="36"/>
+      <c r="AO36" s="36"/>
+    </row>
+    <row r="37" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K37" s="36"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="X37" s="36"/>
+      <c r="AB37" s="36"/>
+      <c r="AE37" s="36"/>
       <c r="AF37" s="36"/>
-      <c r="AG37" s="36"/>
-      <c r="AP37" s="36"/>
-    </row>
-    <row r="38" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L38" s="36"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="Y38" s="36"/>
-      <c r="AC38" s="36"/>
+      <c r="AO37" s="36"/>
+    </row>
+    <row r="38" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K38" s="36"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="X38" s="36"/>
+      <c r="AB38" s="36"/>
+      <c r="AE38" s="36"/>
       <c r="AF38" s="36"/>
-      <c r="AG38" s="36"/>
-      <c r="AP38" s="36"/>
-    </row>
-    <row r="39" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L39" s="36"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48"/>
-      <c r="Y39" s="36"/>
-      <c r="AC39" s="36"/>
+      <c r="AO38" s="36"/>
+    </row>
+    <row r="39" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K39" s="36"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="47"/>
+      <c r="X39" s="36"/>
+      <c r="AB39" s="36"/>
+      <c r="AE39" s="36"/>
       <c r="AF39" s="36"/>
-      <c r="AG39" s="36"/>
-      <c r="AP39" s="36"/>
-    </row>
-    <row r="40" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L40" s="36"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="48"/>
-      <c r="Y40" s="36"/>
-      <c r="AC40" s="36"/>
+      <c r="AO39" s="36"/>
+    </row>
+    <row r="40" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K40" s="36"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="X40" s="36"/>
+      <c r="AB40" s="36"/>
+      <c r="AE40" s="36"/>
       <c r="AF40" s="36"/>
-      <c r="AG40" s="36"/>
-      <c r="AP40" s="36"/>
-    </row>
-    <row r="41" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L41" s="36"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
-      <c r="Y41" s="36"/>
-      <c r="AC41" s="36"/>
+      <c r="AO40" s="36"/>
+    </row>
+    <row r="41" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K41" s="36"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="X41" s="36"/>
+      <c r="AB41" s="36"/>
+      <c r="AE41" s="36"/>
       <c r="AF41" s="36"/>
-      <c r="AG41" s="36"/>
-      <c r="AP41" s="36"/>
-    </row>
-    <row r="42" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L42" s="36"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="Y42" s="36"/>
-      <c r="AC42" s="36"/>
+      <c r="AO41" s="36"/>
+    </row>
+    <row r="42" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K42" s="36"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="X42" s="36"/>
+      <c r="AB42" s="36"/>
+      <c r="AE42" s="36"/>
       <c r="AF42" s="36"/>
-      <c r="AG42" s="36"/>
-      <c r="AP42" s="36"/>
-    </row>
-    <row r="43" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L43" s="36"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="Y43" s="36"/>
-      <c r="AC43" s="36"/>
+      <c r="AO42" s="36"/>
+    </row>
+    <row r="43" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K43" s="36"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="X43" s="36"/>
+      <c r="AB43" s="36"/>
+      <c r="AE43" s="36"/>
       <c r="AF43" s="36"/>
-      <c r="AG43" s="36"/>
-      <c r="AP43" s="36"/>
-    </row>
-    <row r="44" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L44" s="36"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="Y44" s="36"/>
-      <c r="AC44" s="36"/>
+      <c r="AO43" s="36"/>
+    </row>
+    <row r="44" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K44" s="36"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="X44" s="36"/>
+      <c r="AB44" s="36"/>
+      <c r="AE44" s="36"/>
       <c r="AF44" s="36"/>
-      <c r="AG44" s="36"/>
-      <c r="AP44" s="36"/>
-    </row>
-    <row r="45" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L45" s="36"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="Y45" s="36"/>
-      <c r="AC45" s="36"/>
+      <c r="AO44" s="36"/>
+    </row>
+    <row r="45" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K45" s="36"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="X45" s="36"/>
+      <c r="AB45" s="36"/>
+      <c r="AE45" s="36"/>
       <c r="AF45" s="36"/>
-      <c r="AG45" s="36"/>
-      <c r="AP45" s="36"/>
-    </row>
-    <row r="46" spans="12:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L46" s="36"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="Y46" s="36"/>
-      <c r="AC46" s="36"/>
+      <c r="AO45" s="36"/>
+    </row>
+    <row r="46" spans="11:41" ht="18.75" customHeight="1">
+      <c r="K46" s="36"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="X46" s="36"/>
+      <c r="AB46" s="36"/>
+      <c r="AE46" s="36"/>
       <c r="AF46" s="36"/>
-      <c r="AG46" s="36"/>
-      <c r="AP46" s="36"/>
+      <c r="AO46" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3122,27 +3082,27 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="35" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="35" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -3165,11 +3125,11 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="18.75" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>223</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -3272,7 +3232,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="18.75" customHeight="1">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -3373,7 +3333,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="18.75" customHeight="1">
       <c r="A4" t="s">
         <v>339</v>
       </c>
@@ -3471,7 +3431,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="18.75" customHeight="1">
       <c r="D5" s="36"/>
       <c r="M5" s="36"/>
       <c r="Q5" s="36"/>
@@ -3479,7 +3439,7 @@
       <c r="U5" s="36"/>
       <c r="AC5" s="36"/>
     </row>
-    <row r="6" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="18.75" customHeight="1">
       <c r="D6" s="36"/>
       <c r="M6" s="36"/>
       <c r="Q6" s="36"/>
@@ -3487,7 +3447,7 @@
       <c r="U6" s="36"/>
       <c r="AC6" s="36"/>
     </row>
-    <row r="7" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="18.75" customHeight="1">
       <c r="D7" s="36"/>
       <c r="M7" s="36"/>
       <c r="Q7" s="36"/>
@@ -3495,7 +3455,7 @@
       <c r="U7" s="36"/>
       <c r="AC7" s="36"/>
     </row>
-    <row r="8" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="18.75" customHeight="1">
       <c r="A8" s="39" t="s">
         <v>341</v>
       </c>
@@ -3508,7 +3468,7 @@
       <c r="U8" s="36"/>
       <c r="AC8" s="36"/>
     </row>
-    <row r="9" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="18.75" customHeight="1">
       <c r="A9" t="s">
         <v>317</v>
       </c>
@@ -3531,7 +3491,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="18.75" customHeight="1">
       <c r="A10" s="20" t="s">
         <v>222</v>
       </c>
@@ -3638,7 +3598,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="18.75" customHeight="1">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -3686,7 +3646,7 @@
       <c r="U11" s="36"/>
       <c r="AC11" s="36"/>
     </row>
-    <row r="12" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="18.75" customHeight="1">
       <c r="A12" t="s">
         <v>342</v>
       </c>
@@ -3728,7 +3688,7 @@
       <c r="U12" s="36"/>
       <c r="AC12" s="36"/>
     </row>
-    <row r="13" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" ht="18.75" customHeight="1">
       <c r="D13" s="36"/>
       <c r="M13" s="36"/>
       <c r="Q13" s="36"/>
@@ -3736,7 +3696,7 @@
       <c r="U13" s="36"/>
       <c r="AC13" s="36"/>
     </row>
-    <row r="14" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="18.75" customHeight="1">
       <c r="A14" s="39" t="s">
         <v>347</v>
       </c>
@@ -3749,7 +3709,7 @@
       <c r="U14" s="36"/>
       <c r="AC14" s="36"/>
     </row>
-    <row r="15" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="18.75" customHeight="1">
       <c r="A15" t="s">
         <v>317</v>
       </c>
@@ -3772,7 +3732,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="18.75" customHeight="1">
       <c r="A16" s="20" t="s">
         <v>222</v>
       </c>
@@ -3879,7 +3839,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" ht="18.75" customHeight="1">
       <c r="A17" t="s">
         <v>348</v>
       </c>
@@ -3958,7 +3918,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" ht="18.75" customHeight="1">
       <c r="A18" t="s">
         <v>357</v>
       </c>
@@ -4020,7 +3980,7 @@
       </c>
       <c r="AC18" s="36"/>
     </row>
-    <row r="19" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" ht="18.75" customHeight="1">
       <c r="A19" t="s">
         <v>362</v>
       </c>
@@ -4070,7 +4030,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" ht="18.75" customHeight="1">
       <c r="D20" s="36"/>
       <c r="M20" s="36"/>
       <c r="Q20" s="36"/>
@@ -4078,7 +4038,7 @@
       <c r="U20" s="36"/>
       <c r="AC20" s="36"/>
     </row>
-    <row r="21" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="18.75" customHeight="1">
       <c r="D21" s="36"/>
       <c r="M21" s="36"/>
       <c r="Q21" s="36"/>
@@ -4086,7 +4046,7 @@
       <c r="U21" s="36"/>
       <c r="AC21" s="36"/>
     </row>
-    <row r="22" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" ht="18.75" customHeight="1">
       <c r="D22" s="36"/>
       <c r="M22" s="36"/>
       <c r="Q22" s="36"/>
@@ -4094,7 +4054,7 @@
       <c r="U22" s="36"/>
       <c r="AC22" s="36"/>
     </row>
-    <row r="23" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" ht="18.75" customHeight="1">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -4111,7 +4071,7 @@
       <c r="U23" s="36"/>
       <c r="AC23" s="36"/>
     </row>
-    <row r="24" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="18.75" customHeight="1">
       <c r="A24" s="41"/>
       <c r="B24" s="44" t="s">
         <v>367</v>
@@ -4130,7 +4090,7 @@
       <c r="U24" s="36"/>
       <c r="AC24" s="36"/>
     </row>
-    <row r="25" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" ht="18.75" customHeight="1">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
@@ -4147,7 +4107,7 @@
       <c r="U25" s="36"/>
       <c r="AC25" s="36"/>
     </row>
-    <row r="26" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="18.75" customHeight="1">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -4164,7 +4124,7 @@
       <c r="U26" s="36"/>
       <c r="AC26" s="36"/>
     </row>
-    <row r="27" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="18.75" customHeight="1">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -4181,7 +4141,7 @@
       <c r="U27" s="36"/>
       <c r="AC27" s="36"/>
     </row>
-    <row r="28" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="18.75" customHeight="1">
       <c r="D28" s="36"/>
       <c r="M28" s="36"/>
       <c r="Q28" s="36"/>
@@ -4189,7 +4149,7 @@
       <c r="U28" s="36"/>
       <c r="AC28" s="36"/>
     </row>
-    <row r="29" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" ht="18.75" customHeight="1">
       <c r="D29" s="36"/>
       <c r="M29" s="36"/>
       <c r="Q29" s="36"/>
@@ -4197,7 +4157,7 @@
       <c r="U29" s="36"/>
       <c r="AC29" s="36"/>
     </row>
-    <row r="30" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" ht="18.75" customHeight="1">
       <c r="D30" s="36"/>
       <c r="M30" s="36"/>
       <c r="Q30" s="36"/>
@@ -4219,30 +4179,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" ht="18.75" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>222</v>
       </c>
@@ -4364,7 +4324,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" ht="18.75" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>301</v>
       </c>
@@ -4497,24 +4457,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -4609,7 +4569,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="18.75" customHeight="1">
       <c r="A3" t="s">
         <v>278</v>
       </c>
@@ -4692,7 +4652,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="18.75" customHeight="1">
       <c r="O4" s="19"/>
     </row>
   </sheetData>
@@ -4709,20 +4669,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -4817,7 +4777,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1">
       <c r="A2" t="s">
         <v>253</v>
       </c>
@@ -4926,25 +4886,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4954,14 +4914,14 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -4971,14 +4931,14 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4988,14 +4948,14 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -5005,14 +4965,14 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -5022,14 +4982,14 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="50"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -5039,14 +4999,14 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -5056,14 +5016,14 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -5073,14 +5033,14 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="50"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -5090,14 +5050,14 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="50"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -5107,14 +5067,14 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="50"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5124,14 +5084,14 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="50"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5141,14 +5101,14 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="50"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -5158,14 +5118,14 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="50"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -5175,14 +5135,14 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="50"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -5192,14 +5152,14 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="50"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -5209,14 +5169,14 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="18.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -5226,14 +5186,14 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="50"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -5243,14 +5203,14 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -5260,14 +5220,14 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="18.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="50"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -5277,14 +5237,14 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -5294,14 +5254,14 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="50"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -5311,14 +5271,14 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="50"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -5328,14 +5288,14 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="18.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="50"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -5345,7 +5305,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -5360,7 +5320,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="18.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -5377,7 +5337,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="18.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -5394,7 +5354,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -5411,7 +5371,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -5428,7 +5388,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -5445,7 +5405,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="18.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -5460,7 +5420,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="18.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -5477,7 +5437,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -5494,7 +5454,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="18.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -5511,7 +5471,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="18.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
@@ -5526,7 +5486,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="18.75" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -5541,14 +5501,14 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="18.75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="50"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5558,10 +5518,10 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="18.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5571,14 +5531,14 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="18.75" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="51"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -5588,14 +5548,14 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="18.75" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="50"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -5605,14 +5565,14 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="18.75" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="50"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -5622,14 +5582,14 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="18.75" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="50"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -5639,14 +5599,14 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="50"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -5656,14 +5616,14 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="18.75" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="50"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -5673,14 +5633,14 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="18.75" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="50"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -5690,7 +5650,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="18.75" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -5705,7 +5665,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="18.75" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -5720,14 +5680,14 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="18.75" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="49"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -5737,10 +5697,10 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -5750,14 +5710,14 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="18.75" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="50"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -5767,14 +5727,14 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="18.75" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="50"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -5784,14 +5744,14 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="18.75" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="50"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -5801,14 +5761,14 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="18.75" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="50"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -5818,14 +5778,14 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="50"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -5835,14 +5795,14 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="50"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -5852,14 +5812,14 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="50"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -5869,14 +5829,14 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="50"/>
+      <c r="C57" s="49"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -5886,14 +5846,14 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="50"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -5903,14 +5863,14 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B59" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="50"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -5920,14 +5880,14 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="50"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -5937,14 +5897,14 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="50"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -5954,14 +5914,14 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="50" t="s">
+      <c r="B62" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="50"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -5971,14 +5931,14 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="50" t="s">
+      <c r="B63" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="50"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -5988,14 +5948,14 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="50" t="s">
+      <c r="B64" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="50"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -6005,14 +5965,14 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="18.75" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="50"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -6022,14 +5982,14 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="18.75" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B66" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="50"/>
+      <c r="C66" s="49"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -6039,14 +5999,14 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="18.75" customHeight="1">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="50" t="s">
+      <c r="B67" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="50"/>
+      <c r="C67" s="49"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -6056,14 +6016,14 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="18.75" customHeight="1">
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="50" t="s">
+      <c r="B68" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="50"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -6073,14 +6033,14 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="18.75" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="50" t="s">
+      <c r="B69" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="50"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -6090,14 +6050,14 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="50"/>
+      <c r="C70" s="49"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -6107,14 +6067,14 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="18.75" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="50" t="s">
+      <c r="B71" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="50"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -6124,14 +6084,14 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="18.75" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="50"/>
+      <c r="C72" s="49"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -6141,14 +6101,14 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1">
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B73" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="50"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -6158,14 +6118,14 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="18.75" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="50" t="s">
+      <c r="B74" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="50"/>
+      <c r="C74" s="49"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -6175,14 +6135,14 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="18.75" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="50" t="s">
+      <c r="B75" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="50"/>
+      <c r="C75" s="49"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -6192,14 +6152,14 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="18.75" customHeight="1">
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="50" t="s">
+      <c r="B76" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="50"/>
+      <c r="C76" s="49"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -6209,14 +6169,14 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="18.75" customHeight="1">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="50" t="s">
+      <c r="B77" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="50"/>
+      <c r="C77" s="49"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -6226,7 +6186,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="18.75" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>139</v>
       </c>
@@ -6241,7 +6201,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="18.75" customHeight="1">
       <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
@@ -6256,7 +6216,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="18.75" customHeight="1">
       <c r="A80" s="1" t="s">
         <v>141</v>
       </c>
@@ -6273,7 +6233,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="18.75" customHeight="1">
       <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
@@ -6290,7 +6250,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="18.75" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>145</v>
       </c>
@@ -6307,7 +6267,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="18.75" customHeight="1">
       <c r="A83" s="1" t="s">
         <v>147</v>
       </c>
@@ -6324,7 +6284,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="18.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="2"/>
@@ -6337,7 +6297,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="18.75" customHeight="1">
       <c r="A85" s="3" t="s">
         <v>149</v>
       </c>
@@ -6352,7 +6312,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="18.75" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>150</v>
       </c>
@@ -6387,7 +6347,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="18.75" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>153</v>
       </c>
@@ -6422,7 +6382,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="18.75" customHeight="1">
       <c r="A88" s="1" t="s">
         <v>159</v>
       </c>
@@ -6453,7 +6413,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="18.75" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>157</v>
       </c>
@@ -6484,7 +6444,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="18.75" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>154</v>
       </c>
@@ -6513,7 +6473,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="18.75" customHeight="1">
       <c r="A91" s="1" t="s">
         <v>152</v>
       </c>
@@ -6538,7 +6498,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="18.75" customHeight="1">
       <c r="A92" s="1" t="s">
         <v>151</v>
       </c>
@@ -6561,7 +6521,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="18.75" customHeight="1">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -6582,7 +6542,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="18.75" customHeight="1">
       <c r="A94" s="1" t="s">
         <v>158</v>
       </c>
@@ -6601,7 +6561,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="18.75" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>155</v>
       </c>
@@ -6620,7 +6580,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="18.75" customHeight="1">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
@@ -6637,7 +6597,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="18.75" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
@@ -6652,7 +6612,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="18.75" customHeight="1">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
@@ -6667,7 +6627,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="18.75" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
@@ -6682,7 +6642,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="18.75" customHeight="1">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="C100" s="8" t="s">
@@ -6697,7 +6657,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="18.75" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="7" t="s">
@@ -6712,7 +6672,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="18.75" customHeight="1">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
@@ -6727,7 +6687,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="18.75" customHeight="1">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
@@ -6742,7 +6702,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="18.75" customHeight="1">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
@@ -6757,7 +6717,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="18.75" customHeight="1">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1" t="s">
@@ -6772,7 +6732,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="18.75" customHeight="1">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1" t="s">
@@ -6787,7 +6747,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="18.75" customHeight="1">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1" t="s">

</xml_diff>

<commit_message>
added samplesheet check to create some output channels
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA88695A-937D-4718-8E6C-889B728FCFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932D82C4-8544-814E-85CA-52BB031C1A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPXV_Metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="447">
   <si>
     <t>Strategy</t>
   </si>
@@ -1361,6 +1361,24 @@
   </si>
   <si>
     <t>publication_title</t>
+  </si>
+  <si>
+    <t>fasta_path</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/mpox/FL0004.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/mpox/IL0005.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/mpox/NY0006.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/mpox/NY0007.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/mpox/TX0001.fasta</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1388,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1619,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1764,6 +1782,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2070,36 +2094,37 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ46"/>
+  <dimension ref="A1:BA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="37" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.42578125" customWidth="1"/>
-    <col min="39" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.5" customWidth="1"/>
+    <col min="14" max="15" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="29" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" style="17" customWidth="1"/>
+    <col min="32" max="32" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5" customWidth="1"/>
+    <col min="40" max="49" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="13.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -2114,17 +2139,17 @@
       <c r="AB1" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="AE1" s="36" t="s">
+      <c r="AF1" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AG1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AO1" s="36" t="s">
+      <c r="AP1" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1">
+    <row r="2" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>368</v>
       </c>
@@ -2215,71 +2240,74 @@
       <c r="AD2" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="AE2" s="37" t="s">
+      <c r="AE2" s="51" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF2" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="AF2" s="37" t="s">
+      <c r="AG2" s="37" t="s">
         <v>288</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="AL2" s="46" t="s">
+      <c r="AM2" s="46" t="s">
         <v>433</v>
       </c>
-      <c r="AM2" s="46" t="s">
+      <c r="AN2" s="46" t="s">
         <v>298</v>
       </c>
-      <c r="AN2" s="20" t="s">
+      <c r="AO2" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="AO2" s="37" t="s">
+      <c r="AP2" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="AP2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="AQ2" s="20" t="s">
+      <c r="AR2" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AS2" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="AS2" s="20" t="s">
+      <c r="AT2" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="AT2" s="20" t="s">
+      <c r="AU2" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="AU2" s="20" t="s">
+      <c r="AV2" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="AW2" s="21" t="s">
+      <c r="AX2" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="AX2" s="21" t="s">
+      <c r="AY2" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="AY2" s="21" t="s">
+      <c r="AZ2" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="AZ2" s="45" t="s">
+      <c r="BA2" s="45" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18.75" customHeight="1">
+    <row r="3" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -2320,48 +2348,51 @@
       <c r="AD3" s="14">
         <v>247</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="52" t="s">
+        <v>442</v>
+      </c>
+      <c r="AF3" t="s">
         <v>385</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>216</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>4</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>73</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>85</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>310</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>434</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>386</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>387</v>
       </c>
-      <c r="AO3" s="36"/>
-      <c r="AW3" s="14" t="s">
+      <c r="AP3" s="36"/>
+      <c r="AX3" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="AX3" s="17">
+      <c r="AY3" s="17">
         <v>50</v>
       </c>
-      <c r="AY3" s="14">
+      <c r="AZ3" s="14">
         <v>1</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="18.75" customHeight="1">
+    <row r="4" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>389</v>
       </c>
@@ -2399,48 +2430,51 @@
       <c r="AD4" s="14">
         <v>40</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="AF4" t="s">
         <v>395</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>216</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>4</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>73</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>85</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>310</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>434</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>396</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>397</v>
       </c>
-      <c r="AO4" s="36"/>
-      <c r="AW4" s="14">
+      <c r="AP4" s="36"/>
+      <c r="AX4" s="14">
         <v>5</v>
       </c>
-      <c r="AX4" s="16">
+      <c r="AY4" s="16">
         <v>3.5</v>
       </c>
-      <c r="AY4" s="14">
+      <c r="AZ4" s="14">
         <v>0</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BA4" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="18.75" customHeight="1">
+    <row r="5" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>398</v>
       </c>
@@ -2478,48 +2512,51 @@
       <c r="AD5" s="14">
         <v>121</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="AF5" t="s">
         <v>404</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>216</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>73</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>85</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>310</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>434</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>405</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>406</v>
       </c>
-      <c r="AO5" s="36"/>
-      <c r="AW5" s="14">
+      <c r="AP5" s="36"/>
+      <c r="AX5" s="14">
         <v>8</v>
       </c>
-      <c r="AX5" s="14">
+      <c r="AY5" s="14">
         <v>3</v>
       </c>
-      <c r="AY5" s="14">
+      <c r="AZ5" s="14">
         <v>0</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BA5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18.75" customHeight="1">
+    <row r="6" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>407</v>
       </c>
@@ -2560,48 +2597,51 @@
       <c r="AD6" s="14">
         <v>72</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="AF6" t="s">
         <v>411</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>216</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>4</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>73</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>85</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>310</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>434</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>412</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>413</v>
       </c>
-      <c r="AO6" s="36"/>
-      <c r="AW6" s="14">
+      <c r="AP6" s="36"/>
+      <c r="AX6" s="14">
         <v>4</v>
       </c>
-      <c r="AX6" s="16">
+      <c r="AY6" s="16">
         <v>3.2</v>
       </c>
-      <c r="AY6" s="14">
+      <c r="AZ6" s="14">
         <v>1</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BA6" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18.75" customHeight="1">
+    <row r="7" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>414</v>
       </c>
@@ -2642,429 +2682,434 @@
       <c r="AD7" s="14">
         <v>73</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AE7" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="AF7" t="s">
         <v>419</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>216</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>4</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>73</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>85</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>310</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>434</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>420</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>421</v>
       </c>
-      <c r="AO7" s="36"/>
-      <c r="AW7" s="17" t="s">
+      <c r="AP7" s="36"/>
+      <c r="AX7" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="AX7" s="16">
+      <c r="AY7" s="16">
         <v>1.5</v>
       </c>
-      <c r="AY7" s="14">
+      <c r="AZ7" s="14">
         <v>0</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="BA7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18.75" customHeight="1">
+    <row r="8" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X8" s="36"/>
       <c r="AD8" s="14"/>
-      <c r="AO8" s="36"/>
-      <c r="AW8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AP8" s="36"/>
       <c r="AX8" s="14"/>
       <c r="AY8" s="14"/>
-    </row>
-    <row r="9" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AZ8" s="14"/>
+    </row>
+    <row r="9" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X9" s="36"/>
       <c r="AD9" s="14"/>
-      <c r="AO9" s="36"/>
-    </row>
-    <row r="10" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AE9" s="14"/>
+      <c r="AP9" s="36"/>
+    </row>
+    <row r="10" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K10" s="36"/>
       <c r="L10" s="47"/>
       <c r="M10" s="47"/>
       <c r="X10" s="36"/>
       <c r="AB10" s="36"/>
-      <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
-      <c r="AO10" s="36"/>
-    </row>
-    <row r="11" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG10" s="36"/>
+      <c r="AP10" s="36"/>
+    </row>
+    <row r="11" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K11" s="36"/>
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
       <c r="X11" s="36"/>
       <c r="AB11" s="36"/>
-      <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
-      <c r="AO11" s="36"/>
-    </row>
-    <row r="12" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG11" s="36"/>
+      <c r="AP11" s="36"/>
+    </row>
+    <row r="12" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K12" s="36"/>
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
       <c r="X12" s="36"/>
       <c r="AB12" s="36"/>
-      <c r="AE12" s="36"/>
       <c r="AF12" s="36"/>
-      <c r="AO12" s="36"/>
-    </row>
-    <row r="13" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG12" s="36"/>
+      <c r="AP12" s="36"/>
+    </row>
+    <row r="13" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="36"/>
       <c r="L13" s="47"/>
       <c r="M13" s="47"/>
       <c r="X13" s="36"/>
       <c r="AB13" s="36"/>
-      <c r="AE13" s="36"/>
       <c r="AF13" s="36"/>
-      <c r="AO13" s="36"/>
-    </row>
-    <row r="14" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG13" s="36"/>
+      <c r="AP13" s="36"/>
+    </row>
+    <row r="14" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="36"/>
       <c r="L14" s="47"/>
       <c r="M14" s="47"/>
       <c r="X14" s="36"/>
       <c r="AB14" s="36"/>
-      <c r="AE14" s="36"/>
       <c r="AF14" s="36"/>
-      <c r="AO14" s="36"/>
-    </row>
-    <row r="15" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG14" s="36"/>
+      <c r="AP14" s="36"/>
+    </row>
+    <row r="15" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="36"/>
       <c r="L15" s="47"/>
       <c r="M15" s="47"/>
       <c r="X15" s="36"/>
       <c r="AB15" s="36"/>
-      <c r="AE15" s="36"/>
       <c r="AF15" s="36"/>
-      <c r="AO15" s="36"/>
-    </row>
-    <row r="16" spans="1:52" ht="18.75" customHeight="1">
+      <c r="AG15" s="36"/>
+      <c r="AP15" s="36"/>
+    </row>
+    <row r="16" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="36"/>
       <c r="L16" s="47"/>
       <c r="M16" s="47"/>
       <c r="X16" s="36"/>
       <c r="AB16" s="36"/>
-      <c r="AE16" s="36"/>
       <c r="AF16" s="36"/>
-      <c r="AO16" s="36"/>
-    </row>
-    <row r="17" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG16" s="36"/>
+      <c r="AP16" s="36"/>
+    </row>
+    <row r="17" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="36"/>
       <c r="L17" s="47"/>
       <c r="M17" s="47"/>
       <c r="X17" s="36"/>
       <c r="AB17" s="36"/>
-      <c r="AE17" s="36"/>
       <c r="AF17" s="36"/>
-      <c r="AO17" s="36"/>
-    </row>
-    <row r="18" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG17" s="36"/>
+      <c r="AP17" s="36"/>
+    </row>
+    <row r="18" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K18" s="36"/>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
       <c r="X18" s="36"/>
       <c r="AB18" s="36"/>
-      <c r="AE18" s="36"/>
       <c r="AF18" s="36"/>
-      <c r="AO18" s="36"/>
-    </row>
-    <row r="19" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG18" s="36"/>
+      <c r="AP18" s="36"/>
+    </row>
+    <row r="19" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K19" s="36"/>
       <c r="L19" s="47"/>
       <c r="M19" s="47"/>
       <c r="X19" s="36"/>
       <c r="AB19" s="36"/>
-      <c r="AE19" s="36"/>
       <c r="AF19" s="36"/>
-      <c r="AO19" s="36"/>
-    </row>
-    <row r="20" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG19" s="36"/>
+      <c r="AP19" s="36"/>
+    </row>
+    <row r="20" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K20" s="36"/>
       <c r="L20" s="47"/>
       <c r="M20" s="47"/>
       <c r="X20" s="36"/>
       <c r="AB20" s="36"/>
-      <c r="AE20" s="36"/>
       <c r="AF20" s="36"/>
-      <c r="AO20" s="36"/>
-    </row>
-    <row r="21" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG20" s="36"/>
+      <c r="AP20" s="36"/>
+    </row>
+    <row r="21" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K21" s="36"/>
       <c r="L21" s="47"/>
       <c r="M21" s="47"/>
       <c r="X21" s="36"/>
       <c r="AB21" s="36"/>
-      <c r="AE21" s="36"/>
       <c r="AF21" s="36"/>
-      <c r="AO21" s="36"/>
-    </row>
-    <row r="22" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG21" s="36"/>
+      <c r="AP21" s="36"/>
+    </row>
+    <row r="22" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K22" s="36"/>
       <c r="L22" s="47"/>
       <c r="M22" s="47"/>
       <c r="X22" s="36"/>
       <c r="AB22" s="36"/>
-      <c r="AE22" s="36"/>
       <c r="AF22" s="36"/>
-      <c r="AO22" s="36"/>
-    </row>
-    <row r="23" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG22" s="36"/>
+      <c r="AP22" s="36"/>
+    </row>
+    <row r="23" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K23" s="36"/>
       <c r="L23" s="47"/>
       <c r="M23" s="47"/>
       <c r="X23" s="36"/>
       <c r="AB23" s="36"/>
-      <c r="AE23" s="36"/>
       <c r="AF23" s="36"/>
-      <c r="AO23" s="36"/>
-    </row>
-    <row r="24" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG23" s="36"/>
+      <c r="AP23" s="36"/>
+    </row>
+    <row r="24" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K24" s="36"/>
       <c r="L24" s="47"/>
       <c r="M24" s="47"/>
       <c r="X24" s="36"/>
       <c r="AB24" s="36"/>
-      <c r="AE24" s="36"/>
       <c r="AF24" s="36"/>
-      <c r="AO24" s="36"/>
-    </row>
-    <row r="25" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG24" s="36"/>
+      <c r="AP24" s="36"/>
+    </row>
+    <row r="25" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K25" s="36"/>
       <c r="L25" s="47"/>
       <c r="M25" s="47"/>
       <c r="X25" s="36"/>
       <c r="AB25" s="36"/>
-      <c r="AE25" s="36"/>
       <c r="AF25" s="36"/>
-      <c r="AO25" s="36"/>
-    </row>
-    <row r="26" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG25" s="36"/>
+      <c r="AP25" s="36"/>
+    </row>
+    <row r="26" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K26" s="36"/>
       <c r="L26" s="47"/>
       <c r="M26" s="47"/>
       <c r="X26" s="36"/>
       <c r="AB26" s="36"/>
-      <c r="AE26" s="36"/>
       <c r="AF26" s="36"/>
-      <c r="AO26" s="36"/>
-    </row>
-    <row r="27" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG26" s="36"/>
+      <c r="AP26" s="36"/>
+    </row>
+    <row r="27" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K27" s="36"/>
       <c r="L27" s="47"/>
       <c r="M27" s="47"/>
       <c r="X27" s="36"/>
       <c r="AB27" s="36"/>
-      <c r="AE27" s="36"/>
       <c r="AF27" s="36"/>
-      <c r="AO27" s="36"/>
-    </row>
-    <row r="28" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG27" s="36"/>
+      <c r="AP27" s="36"/>
+    </row>
+    <row r="28" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K28" s="36"/>
       <c r="L28" s="47"/>
       <c r="M28" s="47"/>
       <c r="X28" s="36"/>
       <c r="AB28" s="36"/>
-      <c r="AE28" s="36"/>
       <c r="AF28" s="36"/>
-      <c r="AO28" s="36"/>
-    </row>
-    <row r="29" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG28" s="36"/>
+      <c r="AP28" s="36"/>
+    </row>
+    <row r="29" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K29" s="36"/>
       <c r="L29" s="47"/>
       <c r="M29" s="47"/>
       <c r="X29" s="36"/>
       <c r="AB29" s="36"/>
-      <c r="AE29" s="36"/>
       <c r="AF29" s="36"/>
-      <c r="AO29" s="36"/>
-    </row>
-    <row r="30" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG29" s="36"/>
+      <c r="AP29" s="36"/>
+    </row>
+    <row r="30" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K30" s="36"/>
       <c r="L30" s="47"/>
       <c r="M30" s="47"/>
       <c r="X30" s="36"/>
       <c r="AB30" s="36"/>
-      <c r="AE30" s="36"/>
       <c r="AF30" s="36"/>
-      <c r="AO30" s="36"/>
-    </row>
-    <row r="31" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG30" s="36"/>
+      <c r="AP30" s="36"/>
+    </row>
+    <row r="31" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K31" s="36"/>
       <c r="L31" s="47"/>
       <c r="M31" s="47"/>
       <c r="X31" s="36"/>
       <c r="AB31" s="36"/>
-      <c r="AE31" s="36"/>
       <c r="AF31" s="36"/>
-      <c r="AO31" s="36"/>
-    </row>
-    <row r="32" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG31" s="36"/>
+      <c r="AP31" s="36"/>
+    </row>
+    <row r="32" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K32" s="36"/>
       <c r="L32" s="47"/>
       <c r="M32" s="47"/>
       <c r="X32" s="36"/>
       <c r="AB32" s="36"/>
-      <c r="AE32" s="36"/>
       <c r="AF32" s="36"/>
-      <c r="AO32" s="36"/>
-    </row>
-    <row r="33" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG32" s="36"/>
+      <c r="AP32" s="36"/>
+    </row>
+    <row r="33" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K33" s="36"/>
       <c r="L33" s="47"/>
       <c r="M33" s="47"/>
       <c r="X33" s="36"/>
       <c r="AB33" s="36"/>
-      <c r="AE33" s="36"/>
       <c r="AF33" s="36"/>
-      <c r="AO33" s="36"/>
-    </row>
-    <row r="34" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG33" s="36"/>
+      <c r="AP33" s="36"/>
+    </row>
+    <row r="34" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K34" s="36"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
       <c r="X34" s="36"/>
       <c r="AB34" s="36"/>
-      <c r="AE34" s="36"/>
       <c r="AF34" s="36"/>
-      <c r="AO34" s="36"/>
-    </row>
-    <row r="35" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG34" s="36"/>
+      <c r="AP34" s="36"/>
+    </row>
+    <row r="35" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K35" s="36"/>
       <c r="L35" s="47"/>
       <c r="M35" s="47"/>
       <c r="X35" s="36"/>
       <c r="AB35" s="36"/>
-      <c r="AE35" s="36"/>
       <c r="AF35" s="36"/>
-      <c r="AO35" s="36"/>
-    </row>
-    <row r="36" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG35" s="36"/>
+      <c r="AP35" s="36"/>
+    </row>
+    <row r="36" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K36" s="36"/>
       <c r="L36" s="47"/>
       <c r="M36" s="47"/>
       <c r="X36" s="36"/>
       <c r="AB36" s="36"/>
-      <c r="AE36" s="36"/>
       <c r="AF36" s="36"/>
-      <c r="AO36" s="36"/>
-    </row>
-    <row r="37" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG36" s="36"/>
+      <c r="AP36" s="36"/>
+    </row>
+    <row r="37" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K37" s="36"/>
       <c r="L37" s="47"/>
       <c r="M37" s="47"/>
       <c r="X37" s="36"/>
       <c r="AB37" s="36"/>
-      <c r="AE37" s="36"/>
       <c r="AF37" s="36"/>
-      <c r="AO37" s="36"/>
-    </row>
-    <row r="38" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG37" s="36"/>
+      <c r="AP37" s="36"/>
+    </row>
+    <row r="38" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K38" s="36"/>
       <c r="L38" s="47"/>
       <c r="M38" s="47"/>
       <c r="X38" s="36"/>
       <c r="AB38" s="36"/>
-      <c r="AE38" s="36"/>
       <c r="AF38" s="36"/>
-      <c r="AO38" s="36"/>
-    </row>
-    <row r="39" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG38" s="36"/>
+      <c r="AP38" s="36"/>
+    </row>
+    <row r="39" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="36"/>
       <c r="L39" s="47"/>
       <c r="M39" s="47"/>
       <c r="X39" s="36"/>
       <c r="AB39" s="36"/>
-      <c r="AE39" s="36"/>
       <c r="AF39" s="36"/>
-      <c r="AO39" s="36"/>
-    </row>
-    <row r="40" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG39" s="36"/>
+      <c r="AP39" s="36"/>
+    </row>
+    <row r="40" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="36"/>
       <c r="L40" s="47"/>
       <c r="M40" s="47"/>
       <c r="X40" s="36"/>
       <c r="AB40" s="36"/>
-      <c r="AE40" s="36"/>
       <c r="AF40" s="36"/>
-      <c r="AO40" s="36"/>
-    </row>
-    <row r="41" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG40" s="36"/>
+      <c r="AP40" s="36"/>
+    </row>
+    <row r="41" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K41" s="36"/>
       <c r="L41" s="47"/>
       <c r="M41" s="47"/>
       <c r="X41" s="36"/>
       <c r="AB41" s="36"/>
-      <c r="AE41" s="36"/>
       <c r="AF41" s="36"/>
-      <c r="AO41" s="36"/>
-    </row>
-    <row r="42" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG41" s="36"/>
+      <c r="AP41" s="36"/>
+    </row>
+    <row r="42" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K42" s="36"/>
       <c r="L42" s="47"/>
       <c r="M42" s="47"/>
       <c r="X42" s="36"/>
       <c r="AB42" s="36"/>
-      <c r="AE42" s="36"/>
       <c r="AF42" s="36"/>
-      <c r="AO42" s="36"/>
-    </row>
-    <row r="43" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG42" s="36"/>
+      <c r="AP42" s="36"/>
+    </row>
+    <row r="43" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K43" s="36"/>
       <c r="L43" s="47"/>
       <c r="M43" s="47"/>
       <c r="X43" s="36"/>
       <c r="AB43" s="36"/>
-      <c r="AE43" s="36"/>
       <c r="AF43" s="36"/>
-      <c r="AO43" s="36"/>
-    </row>
-    <row r="44" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG43" s="36"/>
+      <c r="AP43" s="36"/>
+    </row>
+    <row r="44" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K44" s="36"/>
       <c r="L44" s="47"/>
       <c r="M44" s="47"/>
       <c r="X44" s="36"/>
       <c r="AB44" s="36"/>
-      <c r="AE44" s="36"/>
       <c r="AF44" s="36"/>
-      <c r="AO44" s="36"/>
-    </row>
-    <row r="45" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG44" s="36"/>
+      <c r="AP44" s="36"/>
+    </row>
+    <row r="45" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K45" s="36"/>
       <c r="L45" s="47"/>
       <c r="M45" s="47"/>
       <c r="X45" s="36"/>
       <c r="AB45" s="36"/>
-      <c r="AE45" s="36"/>
       <c r="AF45" s="36"/>
-      <c r="AO45" s="36"/>
-    </row>
-    <row r="46" spans="11:41" ht="18.75" customHeight="1">
+      <c r="AG45" s="36"/>
+      <c r="AP45" s="36"/>
+    </row>
+    <row r="46" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K46" s="36"/>
       <c r="L46" s="47"/>
       <c r="M46" s="47"/>
       <c r="X46" s="36"/>
       <c r="AB46" s="36"/>
-      <c r="AE46" s="36"/>
       <c r="AF46" s="36"/>
-      <c r="AO46" s="36"/>
+      <c r="AG46" s="36"/>
+      <c r="AP46" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3082,27 +3127,27 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="35" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="35" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -3125,7 +3170,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18.75" customHeight="1">
+    <row r="2" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>222</v>
       </c>
@@ -3232,7 +3277,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="18.75" customHeight="1">
+    <row r="3" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -3333,7 +3378,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="18.75" customHeight="1">
+    <row r="4" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>339</v>
       </c>
@@ -3431,7 +3476,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="18.75" customHeight="1">
+    <row r="5" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="36"/>
       <c r="M5" s="36"/>
       <c r="Q5" s="36"/>
@@ -3439,7 +3484,7 @@
       <c r="U5" s="36"/>
       <c r="AC5" s="36"/>
     </row>
-    <row r="6" spans="1:35" ht="18.75" customHeight="1">
+    <row r="6" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="36"/>
       <c r="M6" s="36"/>
       <c r="Q6" s="36"/>
@@ -3447,7 +3492,7 @@
       <c r="U6" s="36"/>
       <c r="AC6" s="36"/>
     </row>
-    <row r="7" spans="1:35" ht="18.75" customHeight="1">
+    <row r="7" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="36"/>
       <c r="M7" s="36"/>
       <c r="Q7" s="36"/>
@@ -3455,7 +3500,7 @@
       <c r="U7" s="36"/>
       <c r="AC7" s="36"/>
     </row>
-    <row r="8" spans="1:35" ht="18.75" customHeight="1">
+    <row r="8" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
         <v>341</v>
       </c>
@@ -3468,7 +3513,7 @@
       <c r="U8" s="36"/>
       <c r="AC8" s="36"/>
     </row>
-    <row r="9" spans="1:35" ht="18.75" customHeight="1">
+    <row r="9" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>317</v>
       </c>
@@ -3491,7 +3536,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="18.75" customHeight="1">
+    <row r="10" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>222</v>
       </c>
@@ -3598,7 +3643,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="18.75" customHeight="1">
+    <row r="11" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -3646,7 +3691,7 @@
       <c r="U11" s="36"/>
       <c r="AC11" s="36"/>
     </row>
-    <row r="12" spans="1:35" ht="18.75" customHeight="1">
+    <row r="12" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>342</v>
       </c>
@@ -3688,7 +3733,7 @@
       <c r="U12" s="36"/>
       <c r="AC12" s="36"/>
     </row>
-    <row r="13" spans="1:35" ht="18.75" customHeight="1">
+    <row r="13" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="36"/>
       <c r="M13" s="36"/>
       <c r="Q13" s="36"/>
@@ -3696,7 +3741,7 @@
       <c r="U13" s="36"/>
       <c r="AC13" s="36"/>
     </row>
-    <row r="14" spans="1:35" ht="18.75" customHeight="1">
+    <row r="14" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
         <v>347</v>
       </c>
@@ -3709,7 +3754,7 @@
       <c r="U14" s="36"/>
       <c r="AC14" s="36"/>
     </row>
-    <row r="15" spans="1:35" ht="18.75" customHeight="1">
+    <row r="15" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>317</v>
       </c>
@@ -3732,7 +3777,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="18.75" customHeight="1">
+    <row r="16" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>222</v>
       </c>
@@ -3839,7 +3884,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="18.75" customHeight="1">
+    <row r="17" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>348</v>
       </c>
@@ -3918,7 +3963,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="18.75" customHeight="1">
+    <row r="18" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>357</v>
       </c>
@@ -3980,7 +4025,7 @@
       </c>
       <c r="AC18" s="36"/>
     </row>
-    <row r="19" spans="1:35" ht="18.75" customHeight="1">
+    <row r="19" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>362</v>
       </c>
@@ -4030,7 +4075,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="18.75" customHeight="1">
+    <row r="20" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="36"/>
       <c r="M20" s="36"/>
       <c r="Q20" s="36"/>
@@ -4038,7 +4083,7 @@
       <c r="U20" s="36"/>
       <c r="AC20" s="36"/>
     </row>
-    <row r="21" spans="1:35" ht="18.75" customHeight="1">
+    <row r="21" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="36"/>
       <c r="M21" s="36"/>
       <c r="Q21" s="36"/>
@@ -4046,7 +4091,7 @@
       <c r="U21" s="36"/>
       <c r="AC21" s="36"/>
     </row>
-    <row r="22" spans="1:35" ht="18.75" customHeight="1">
+    <row r="22" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="36"/>
       <c r="M22" s="36"/>
       <c r="Q22" s="36"/>
@@ -4054,7 +4099,7 @@
       <c r="U22" s="36"/>
       <c r="AC22" s="36"/>
     </row>
-    <row r="23" spans="1:35" ht="18.75" customHeight="1">
+    <row r="23" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -4071,7 +4116,7 @@
       <c r="U23" s="36"/>
       <c r="AC23" s="36"/>
     </row>
-    <row r="24" spans="1:35" ht="18.75" customHeight="1">
+    <row r="24" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="44" t="s">
         <v>367</v>
@@ -4090,7 +4135,7 @@
       <c r="U24" s="36"/>
       <c r="AC24" s="36"/>
     </row>
-    <row r="25" spans="1:35" ht="18.75" customHeight="1">
+    <row r="25" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
@@ -4107,7 +4152,7 @@
       <c r="U25" s="36"/>
       <c r="AC25" s="36"/>
     </row>
-    <row r="26" spans="1:35" ht="18.75" customHeight="1">
+    <row r="26" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -4124,7 +4169,7 @@
       <c r="U26" s="36"/>
       <c r="AC26" s="36"/>
     </row>
-    <row r="27" spans="1:35" ht="18.75" customHeight="1">
+    <row r="27" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -4141,7 +4186,7 @@
       <c r="U27" s="36"/>
       <c r="AC27" s="36"/>
     </row>
-    <row r="28" spans="1:35" ht="18.75" customHeight="1">
+    <row r="28" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="36"/>
       <c r="M28" s="36"/>
       <c r="Q28" s="36"/>
@@ -4149,7 +4194,7 @@
       <c r="U28" s="36"/>
       <c r="AC28" s="36"/>
     </row>
-    <row r="29" spans="1:35" ht="18.75" customHeight="1">
+    <row r="29" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="36"/>
       <c r="M29" s="36"/>
       <c r="Q29" s="36"/>
@@ -4157,7 +4202,7 @@
       <c r="U29" s="36"/>
       <c r="AC29" s="36"/>
     </row>
-    <row r="30" spans="1:35" ht="18.75" customHeight="1">
+    <row r="30" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="36"/>
       <c r="M30" s="36"/>
       <c r="Q30" s="36"/>
@@ -4179,30 +4224,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75" customHeight="1">
+    <row r="1" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>222</v>
       </c>
@@ -4324,7 +4369,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="18.75" customHeight="1">
+    <row r="2" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>301</v>
       </c>
@@ -4457,24 +4502,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -4569,7 +4614,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18.75" customHeight="1">
+    <row r="3" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>278</v>
       </c>
@@ -4652,7 +4697,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="18.75" customHeight="1">
+    <row r="4" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O4" s="19"/>
     </row>
   </sheetData>
@@ -4669,20 +4714,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="31" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -4777,7 +4822,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="18.75" customHeight="1">
+    <row r="2" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>253</v>
       </c>
@@ -4886,22 +4931,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4914,7 +4959,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4931,7 +4976,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4948,7 +4993,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4965,7 +5010,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -4982,7 +5027,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -4999,7 +5044,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -5016,7 +5061,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -5033,7 +5078,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -5050,7 +5095,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -5067,7 +5112,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -5084,7 +5129,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -5101,7 +5146,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -5118,7 +5163,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -5135,7 +5180,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -5152,7 +5197,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -5169,7 +5214,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="18.75" customHeight="1">
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -5186,7 +5231,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -5203,7 +5248,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -5220,7 +5265,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1">
+    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -5237,7 +5282,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -5254,7 +5299,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -5271,7 +5316,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -5288,7 +5333,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1">
+    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -5305,7 +5350,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -5320,7 +5365,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1">
+    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -5337,7 +5382,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1">
+    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -5354,7 +5399,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -5371,7 +5416,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -5388,7 +5433,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -5405,7 +5450,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="18.75" customHeight="1">
+    <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -5420,7 +5465,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="18.75" customHeight="1">
+    <row r="32" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -5437,7 +5482,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="18.75" customHeight="1">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -5454,7 +5499,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="18.75" customHeight="1">
+    <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -5471,7 +5516,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="18.75" customHeight="1">
+    <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
@@ -5486,7 +5531,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="18.75" customHeight="1">
+    <row r="36" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -5501,7 +5546,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="18.75" customHeight="1">
+    <row r="37" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -5518,7 +5563,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="18.75" customHeight="1">
+    <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="49"/>
       <c r="C38" s="49"/>
@@ -5531,7 +5576,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="18.75" customHeight="1">
+    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
@@ -5548,7 +5593,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="18.75" customHeight="1">
+    <row r="40" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
@@ -5565,7 +5610,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="18.75" customHeight="1">
+    <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
@@ -5582,7 +5627,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="18.75" customHeight="1">
+    <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
@@ -5599,7 +5644,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="18.75" customHeight="1">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
@@ -5616,7 +5661,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="18.75" customHeight="1">
+    <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
@@ -5633,7 +5678,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="18.75" customHeight="1">
+    <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
@@ -5650,7 +5695,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="18.75" customHeight="1">
+    <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -5665,7 +5710,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="18.75" customHeight="1">
+    <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -5680,7 +5725,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="18.75" customHeight="1">
+    <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -5697,7 +5742,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="18.75" customHeight="1">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="49"/>
       <c r="C49" s="49"/>
@@ -5710,7 +5755,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="18.75" customHeight="1">
+    <row r="50" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -5727,7 +5772,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="18.75" customHeight="1">
+    <row r="51" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -5744,7 +5789,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="18.75" customHeight="1">
+    <row r="52" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
@@ -5761,7 +5806,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="18.75" customHeight="1">
+    <row r="53" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
@@ -5778,7 +5823,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="18.75" customHeight="1">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
@@ -5795,7 +5840,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="18.75" customHeight="1">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
@@ -5812,7 +5857,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="18.75" customHeight="1">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
@@ -5829,7 +5874,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="18.75" customHeight="1">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -5846,7 +5891,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="18.75" customHeight="1">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -5863,7 +5908,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="18.75" customHeight="1">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
@@ -5880,7 +5925,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="18.75" customHeight="1">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
@@ -5897,7 +5942,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="18.75" customHeight="1">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
@@ -5914,7 +5959,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" ht="18.75" customHeight="1">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -5931,7 +5976,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="18.75" customHeight="1">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
@@ -5948,7 +5993,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="18.75" customHeight="1">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
@@ -5965,7 +6010,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" ht="18.75" customHeight="1">
+    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
@@ -5982,7 +6027,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="18.75" customHeight="1">
+    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
@@ -5999,7 +6044,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" ht="18.75" customHeight="1">
+    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
@@ -6016,7 +6061,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="18.75" customHeight="1">
+    <row r="68" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
@@ -6033,7 +6078,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" ht="18.75" customHeight="1">
+    <row r="69" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
@@ -6050,7 +6095,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" ht="18.75" customHeight="1">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
@@ -6067,7 +6112,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" ht="18.75" customHeight="1">
+    <row r="71" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
@@ -6084,7 +6129,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="18.75" customHeight="1">
+    <row r="72" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
@@ -6101,7 +6146,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" ht="18.75" customHeight="1">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
@@ -6118,7 +6163,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" ht="18.75" customHeight="1">
+    <row r="74" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
@@ -6135,7 +6180,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" ht="18.75" customHeight="1">
+    <row r="75" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
@@ -6152,7 +6197,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" ht="18.75" customHeight="1">
+    <row r="76" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
@@ -6169,7 +6214,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" ht="18.75" customHeight="1">
+    <row r="77" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
@@ -6186,7 +6231,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" ht="18.75" customHeight="1">
+    <row r="78" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>139</v>
       </c>
@@ -6201,7 +6246,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="18.75" customHeight="1">
+    <row r="79" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
@@ -6216,7 +6261,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="18.75" customHeight="1">
+    <row r="80" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>141</v>
       </c>
@@ -6233,7 +6278,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" ht="18.75" customHeight="1">
+    <row r="81" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
@@ -6250,7 +6295,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" ht="18.75" customHeight="1">
+    <row r="82" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>145</v>
       </c>
@@ -6267,7 +6312,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="18.75" customHeight="1">
+    <row r="83" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>147</v>
       </c>
@@ -6284,7 +6329,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" ht="18.75" customHeight="1">
+    <row r="84" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="2"/>
@@ -6297,7 +6342,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" ht="18.75" customHeight="1">
+    <row r="85" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>149</v>
       </c>
@@ -6312,7 +6357,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" ht="18.75" customHeight="1">
+    <row r="86" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>150</v>
       </c>
@@ -6347,7 +6392,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="18.75" customHeight="1">
+    <row r="87" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>153</v>
       </c>
@@ -6382,7 +6427,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="18.75" customHeight="1">
+    <row r="88" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>159</v>
       </c>
@@ -6413,7 +6458,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="18.75" customHeight="1">
+    <row r="89" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>157</v>
       </c>
@@ -6444,7 +6489,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18.75" customHeight="1">
+    <row r="90" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>154</v>
       </c>
@@ -6473,7 +6518,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18.75" customHeight="1">
+    <row r="91" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>152</v>
       </c>
@@ -6498,7 +6543,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="18.75" customHeight="1">
+    <row r="92" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>151</v>
       </c>
@@ -6521,7 +6566,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="18.75" customHeight="1">
+    <row r="93" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -6542,7 +6587,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="18.75" customHeight="1">
+    <row r="94" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>158</v>
       </c>
@@ -6561,7 +6606,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" ht="18.75" customHeight="1">
+    <row r="95" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>155</v>
       </c>
@@ -6580,7 +6625,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" ht="18.75" customHeight="1">
+    <row r="96" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
@@ -6597,7 +6642,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" ht="18.75" customHeight="1">
+    <row r="97" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
@@ -6612,7 +6657,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" ht="18.75" customHeight="1">
+    <row r="98" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
@@ -6627,7 +6672,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" ht="18.75" customHeight="1">
+    <row r="99" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
@@ -6642,7 +6687,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" ht="18.75" customHeight="1">
+    <row r="100" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="C100" s="8" t="s">
@@ -6657,7 +6702,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" ht="18.75" customHeight="1">
+    <row r="101" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="7" t="s">
@@ -6672,7 +6717,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" ht="18.75" customHeight="1">
+    <row r="102" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
@@ -6687,7 +6732,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" ht="18.75" customHeight="1">
+    <row r="103" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
@@ -6702,7 +6747,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" ht="18.75" customHeight="1">
+    <row r="104" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
@@ -6717,7 +6762,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" ht="18.75" customHeight="1">
+    <row r="105" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1" t="s">
@@ -6732,7 +6777,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" ht="18.75" customHeight="1">
+    <row r="106" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1" t="s">
@@ -6747,7 +6792,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" ht="18.75" customHeight="1">
+    <row r="107" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1" t="s">
@@ -6764,61 +6809,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6827,6 +6817,61 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gffs for viral mpox workflow to test user provided annotations. Also simplified submission part of main workflow.
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/custom_fields_MPXV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A47A121-6CD1-5642-BD70-0CEC0274E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE30C83-3DA3-A94D-B624-C6F9541C9F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="445">
   <si>
     <t>Strategy</t>
   </si>
@@ -1370,6 +1370,9 @@
   </si>
   <si>
     <t>FL0004</t>
+  </si>
+  <si>
+    <t>gff_path</t>
   </si>
 </sst>
 </file>
@@ -2085,10 +2088,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AY45"/>
+  <dimension ref="A1:AZ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AM17" sqref="AM17"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2107,15 +2110,15 @@
     <col min="20" max="21" width="19.5" bestFit="1" customWidth="1"/>
     <col min="22" max="29" width="13.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.5" style="17" customWidth="1"/>
-    <col min="32" max="32" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5" customWidth="1"/>
-    <col min="40" max="48" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="13.5" style="17" customWidth="1"/>
+    <col min="33" max="33" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="39" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5" customWidth="1"/>
+    <col min="41" max="49" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="13.5" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -2130,17 +2133,17 @@
       <c r="AB1" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AG1" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="AG1" s="36" t="s">
+      <c r="AH1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AP1" s="36" t="s">
+      <c r="AQ1" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
         <v>441</v>
       </c>
@@ -2234,68 +2237,71 @@
       <c r="AE2" s="48" t="s">
         <v>422</v>
       </c>
-      <c r="AF2" s="37" t="s">
+      <c r="AF2" s="48" t="s">
+        <v>444</v>
+      </c>
+      <c r="AG2" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="AG2" s="37" t="s">
+      <c r="AH2" s="37" t="s">
         <v>288</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AM2" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="AM2" s="45" t="s">
+      <c r="AN2" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="AN2" s="45" t="s">
+      <c r="AO2" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AO2" s="20" t="s">
+      <c r="AP2" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="AP2" s="37" t="s">
+      <c r="AQ2" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="AQ2" s="20" t="s">
+      <c r="AR2" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AS2" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="AS2" s="20" t="s">
+      <c r="AT2" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="AT2" s="20" t="s">
+      <c r="AU2" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="AU2" s="20" t="s">
+      <c r="AV2" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="AV2" s="20" t="s">
+      <c r="AW2" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="AW2" s="21" t="s">
+      <c r="AX2" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="AX2" s="21" t="s">
+      <c r="AY2" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="AY2" s="21" t="s">
+      <c r="AZ2" s="21" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>385</v>
       </c>
@@ -2336,45 +2342,46 @@
       <c r="AE3" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="14"/>
+      <c r="AG3" t="s">
         <v>391</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>216</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>73</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>85</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>310</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>415</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>429</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>434</v>
       </c>
-      <c r="AP3" s="36"/>
-      <c r="AW3" s="14">
+      <c r="AQ3" s="36"/>
+      <c r="AX3" s="14">
         <v>5</v>
       </c>
-      <c r="AX3" s="50" t="s">
+      <c r="AY3" s="50" t="s">
         <v>438</v>
       </c>
-      <c r="AY3" s="14">
+      <c r="AZ3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -2415,45 +2422,46 @@
       <c r="AE4" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="14"/>
+      <c r="AG4" t="s">
         <v>398</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>216</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>73</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>85</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>310</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>415</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>430</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>435</v>
       </c>
-      <c r="AP4" s="36"/>
-      <c r="AW4" s="14">
+      <c r="AQ4" s="36"/>
+      <c r="AX4" s="14">
         <v>8</v>
       </c>
-      <c r="AX4" s="49" t="s">
+      <c r="AY4" s="49" t="s">
         <v>439</v>
       </c>
-      <c r="AY4" s="14">
+      <c r="AZ4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -2497,45 +2505,46 @@
       <c r="AE5" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" s="14"/>
+      <c r="AG5" t="s">
         <v>403</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>216</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>4</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>73</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>85</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>310</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>415</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>431</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>436</v>
       </c>
-      <c r="AP5" s="36"/>
-      <c r="AW5" s="14">
+      <c r="AQ5" s="36"/>
+      <c r="AX5" s="14">
         <v>4</v>
       </c>
-      <c r="AX5" s="50" t="s">
+      <c r="AY5" s="50" t="s">
         <v>440</v>
       </c>
-      <c r="AY5" s="14">
+      <c r="AZ5" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>442</v>
       </c>
@@ -2579,45 +2588,46 @@
       <c r="AE6" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AF6" s="14"/>
+      <c r="AG6" t="s">
         <v>408</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>216</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>4</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>73</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>85</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>310</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>415</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>432</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>437</v>
       </c>
-      <c r="AP6" s="36"/>
-      <c r="AW6" s="17" t="s">
+      <c r="AQ6" s="36"/>
+      <c r="AX6" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="AX6" s="50" t="s">
+      <c r="AY6" s="50" t="s">
         <v>406</v>
       </c>
-      <c r="AY6" s="14">
+      <c r="AZ6" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>443</v>
       </c>
@@ -2661,419 +2671,421 @@
       <c r="AE7" s="49" t="s">
         <v>423</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AF7" s="49"/>
+      <c r="AG7" t="s">
         <v>383</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>216</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>4</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>73</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>85</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>310</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>415</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>428</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>433</v>
       </c>
-      <c r="AP7" s="36"/>
-      <c r="AW7" s="14" t="s">
+      <c r="AQ7" s="36"/>
+      <c r="AX7" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="AX7" s="17" t="s">
+      <c r="AY7" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="AY7" s="14">
+      <c r="AZ7" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="X8" s="36"/>
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
-      <c r="AP8" s="36"/>
-    </row>
-    <row r="9" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF8" s="14"/>
+      <c r="AQ8" s="36"/>
+    </row>
+    <row r="9" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K9" s="36"/>
       <c r="L9" s="46"/>
       <c r="M9" s="46"/>
       <c r="X9" s="36"/>
       <c r="AB9" s="36"/>
-      <c r="AF9" s="36"/>
       <c r="AG9" s="36"/>
-      <c r="AP9" s="36"/>
-    </row>
-    <row r="10" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH9" s="36"/>
+      <c r="AQ9" s="36"/>
+    </row>
+    <row r="10" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K10" s="36"/>
       <c r="L10" s="46"/>
       <c r="M10" s="46"/>
       <c r="X10" s="36"/>
       <c r="AB10" s="36"/>
-      <c r="AF10" s="36"/>
       <c r="AG10" s="36"/>
-      <c r="AP10" s="36"/>
-    </row>
-    <row r="11" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH10" s="36"/>
+      <c r="AQ10" s="36"/>
+    </row>
+    <row r="11" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K11" s="36"/>
       <c r="L11" s="46"/>
       <c r="M11" s="46"/>
       <c r="X11" s="36"/>
       <c r="AB11" s="36"/>
-      <c r="AF11" s="36"/>
       <c r="AG11" s="36"/>
-      <c r="AP11" s="36"/>
-    </row>
-    <row r="12" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH11" s="36"/>
+      <c r="AQ11" s="36"/>
+    </row>
+    <row r="12" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K12" s="36"/>
       <c r="L12" s="46"/>
       <c r="M12" s="46"/>
       <c r="X12" s="36"/>
       <c r="AB12" s="36"/>
-      <c r="AF12" s="36"/>
       <c r="AG12" s="36"/>
-      <c r="AP12" s="36"/>
-    </row>
-    <row r="13" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH12" s="36"/>
+      <c r="AQ12" s="36"/>
+    </row>
+    <row r="13" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="36"/>
       <c r="L13" s="46"/>
       <c r="M13" s="46"/>
       <c r="X13" s="36"/>
       <c r="AB13" s="36"/>
-      <c r="AF13" s="36"/>
       <c r="AG13" s="36"/>
-      <c r="AP13" s="36"/>
-    </row>
-    <row r="14" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH13" s="36"/>
+      <c r="AQ13" s="36"/>
+    </row>
+    <row r="14" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="36"/>
       <c r="L14" s="46"/>
       <c r="M14" s="46"/>
       <c r="X14" s="36"/>
       <c r="AB14" s="36"/>
-      <c r="AF14" s="36"/>
       <c r="AG14" s="36"/>
-      <c r="AP14" s="36"/>
-    </row>
-    <row r="15" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH14" s="36"/>
+      <c r="AQ14" s="36"/>
+    </row>
+    <row r="15" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="36"/>
       <c r="L15" s="46"/>
       <c r="M15" s="46"/>
       <c r="X15" s="36"/>
       <c r="AB15" s="36"/>
-      <c r="AF15" s="36"/>
       <c r="AG15" s="36"/>
-      <c r="AP15" s="36"/>
-    </row>
-    <row r="16" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH15" s="36"/>
+      <c r="AQ15" s="36"/>
+    </row>
+    <row r="16" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="36"/>
       <c r="L16" s="46"/>
       <c r="M16" s="46"/>
       <c r="X16" s="36"/>
       <c r="AB16" s="36"/>
-      <c r="AF16" s="36"/>
       <c r="AG16" s="36"/>
-      <c r="AP16" s="36"/>
-    </row>
-    <row r="17" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH16" s="36"/>
+      <c r="AQ16" s="36"/>
+    </row>
+    <row r="17" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="36"/>
       <c r="L17" s="46"/>
       <c r="M17" s="46"/>
       <c r="X17" s="36"/>
       <c r="AB17" s="36"/>
-      <c r="AF17" s="36"/>
       <c r="AG17" s="36"/>
-      <c r="AP17" s="36"/>
-    </row>
-    <row r="18" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH17" s="36"/>
+      <c r="AQ17" s="36"/>
+    </row>
+    <row r="18" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K18" s="36"/>
       <c r="L18" s="46"/>
       <c r="M18" s="46"/>
       <c r="X18" s="36"/>
       <c r="AB18" s="36"/>
-      <c r="AF18" s="36"/>
       <c r="AG18" s="36"/>
-      <c r="AP18" s="36"/>
-    </row>
-    <row r="19" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH18" s="36"/>
+      <c r="AQ18" s="36"/>
+    </row>
+    <row r="19" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K19" s="36"/>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
       <c r="X19" s="36"/>
       <c r="AB19" s="36"/>
-      <c r="AF19" s="36"/>
       <c r="AG19" s="36"/>
-      <c r="AP19" s="36"/>
-    </row>
-    <row r="20" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH19" s="36"/>
+      <c r="AQ19" s="36"/>
+    </row>
+    <row r="20" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K20" s="36"/>
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
       <c r="X20" s="36"/>
       <c r="AB20" s="36"/>
-      <c r="AF20" s="36"/>
       <c r="AG20" s="36"/>
-      <c r="AP20" s="36"/>
-    </row>
-    <row r="21" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH20" s="36"/>
+      <c r="AQ20" s="36"/>
+    </row>
+    <row r="21" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K21" s="36"/>
       <c r="L21" s="46"/>
       <c r="M21" s="46"/>
       <c r="X21" s="36"/>
       <c r="AB21" s="36"/>
-      <c r="AF21" s="36"/>
       <c r="AG21" s="36"/>
-      <c r="AP21" s="36"/>
-    </row>
-    <row r="22" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH21" s="36"/>
+      <c r="AQ21" s="36"/>
+    </row>
+    <row r="22" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K22" s="36"/>
       <c r="L22" s="46"/>
       <c r="M22" s="46"/>
       <c r="X22" s="36"/>
       <c r="AB22" s="36"/>
-      <c r="AF22" s="36"/>
       <c r="AG22" s="36"/>
-      <c r="AP22" s="36"/>
-    </row>
-    <row r="23" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH22" s="36"/>
+      <c r="AQ22" s="36"/>
+    </row>
+    <row r="23" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K23" s="36"/>
       <c r="L23" s="46"/>
       <c r="M23" s="46"/>
       <c r="X23" s="36"/>
       <c r="AB23" s="36"/>
-      <c r="AF23" s="36"/>
       <c r="AG23" s="36"/>
-      <c r="AP23" s="36"/>
-    </row>
-    <row r="24" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH23" s="36"/>
+      <c r="AQ23" s="36"/>
+    </row>
+    <row r="24" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K24" s="36"/>
       <c r="L24" s="46"/>
       <c r="M24" s="46"/>
       <c r="X24" s="36"/>
       <c r="AB24" s="36"/>
-      <c r="AF24" s="36"/>
       <c r="AG24" s="36"/>
-      <c r="AP24" s="36"/>
-    </row>
-    <row r="25" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH24" s="36"/>
+      <c r="AQ24" s="36"/>
+    </row>
+    <row r="25" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K25" s="36"/>
       <c r="L25" s="46"/>
       <c r="M25" s="46"/>
       <c r="X25" s="36"/>
       <c r="AB25" s="36"/>
-      <c r="AF25" s="36"/>
       <c r="AG25" s="36"/>
-      <c r="AP25" s="36"/>
-    </row>
-    <row r="26" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH25" s="36"/>
+      <c r="AQ25" s="36"/>
+    </row>
+    <row r="26" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K26" s="36"/>
       <c r="L26" s="46"/>
       <c r="M26" s="46"/>
       <c r="X26" s="36"/>
       <c r="AB26" s="36"/>
-      <c r="AF26" s="36"/>
       <c r="AG26" s="36"/>
-      <c r="AP26" s="36"/>
-    </row>
-    <row r="27" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH26" s="36"/>
+      <c r="AQ26" s="36"/>
+    </row>
+    <row r="27" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K27" s="36"/>
       <c r="L27" s="46"/>
       <c r="M27" s="46"/>
       <c r="X27" s="36"/>
       <c r="AB27" s="36"/>
-      <c r="AF27" s="36"/>
       <c r="AG27" s="36"/>
-      <c r="AP27" s="36"/>
-    </row>
-    <row r="28" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH27" s="36"/>
+      <c r="AQ27" s="36"/>
+    </row>
+    <row r="28" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K28" s="36"/>
       <c r="L28" s="46"/>
       <c r="M28" s="46"/>
       <c r="X28" s="36"/>
       <c r="AB28" s="36"/>
-      <c r="AF28" s="36"/>
       <c r="AG28" s="36"/>
-      <c r="AP28" s="36"/>
-    </row>
-    <row r="29" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH28" s="36"/>
+      <c r="AQ28" s="36"/>
+    </row>
+    <row r="29" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K29" s="36"/>
       <c r="L29" s="46"/>
       <c r="M29" s="46"/>
       <c r="X29" s="36"/>
       <c r="AB29" s="36"/>
-      <c r="AF29" s="36"/>
       <c r="AG29" s="36"/>
-      <c r="AP29" s="36"/>
-    </row>
-    <row r="30" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH29" s="36"/>
+      <c r="AQ29" s="36"/>
+    </row>
+    <row r="30" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K30" s="36"/>
       <c r="L30" s="46"/>
       <c r="M30" s="46"/>
       <c r="X30" s="36"/>
       <c r="AB30" s="36"/>
-      <c r="AF30" s="36"/>
       <c r="AG30" s="36"/>
-      <c r="AP30" s="36"/>
-    </row>
-    <row r="31" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH30" s="36"/>
+      <c r="AQ30" s="36"/>
+    </row>
+    <row r="31" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K31" s="36"/>
       <c r="L31" s="46"/>
       <c r="M31" s="46"/>
       <c r="X31" s="36"/>
       <c r="AB31" s="36"/>
-      <c r="AF31" s="36"/>
       <c r="AG31" s="36"/>
-      <c r="AP31" s="36"/>
-    </row>
-    <row r="32" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH31" s="36"/>
+      <c r="AQ31" s="36"/>
+    </row>
+    <row r="32" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K32" s="36"/>
       <c r="L32" s="46"/>
       <c r="M32" s="46"/>
       <c r="X32" s="36"/>
       <c r="AB32" s="36"/>
-      <c r="AF32" s="36"/>
       <c r="AG32" s="36"/>
-      <c r="AP32" s="36"/>
-    </row>
-    <row r="33" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH32" s="36"/>
+      <c r="AQ32" s="36"/>
+    </row>
+    <row r="33" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K33" s="36"/>
       <c r="L33" s="46"/>
       <c r="M33" s="46"/>
       <c r="X33" s="36"/>
       <c r="AB33" s="36"/>
-      <c r="AF33" s="36"/>
       <c r="AG33" s="36"/>
-      <c r="AP33" s="36"/>
-    </row>
-    <row r="34" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH33" s="36"/>
+      <c r="AQ33" s="36"/>
+    </row>
+    <row r="34" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K34" s="36"/>
       <c r="L34" s="46"/>
       <c r="M34" s="46"/>
       <c r="X34" s="36"/>
       <c r="AB34" s="36"/>
-      <c r="AF34" s="36"/>
       <c r="AG34" s="36"/>
-      <c r="AP34" s="36"/>
-    </row>
-    <row r="35" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH34" s="36"/>
+      <c r="AQ34" s="36"/>
+    </row>
+    <row r="35" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K35" s="36"/>
       <c r="L35" s="46"/>
       <c r="M35" s="46"/>
       <c r="X35" s="36"/>
       <c r="AB35" s="36"/>
-      <c r="AF35" s="36"/>
       <c r="AG35" s="36"/>
-      <c r="AP35" s="36"/>
-    </row>
-    <row r="36" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH35" s="36"/>
+      <c r="AQ35" s="36"/>
+    </row>
+    <row r="36" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K36" s="36"/>
       <c r="L36" s="46"/>
       <c r="M36" s="46"/>
       <c r="X36" s="36"/>
       <c r="AB36" s="36"/>
-      <c r="AF36" s="36"/>
       <c r="AG36" s="36"/>
-      <c r="AP36" s="36"/>
-    </row>
-    <row r="37" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH36" s="36"/>
+      <c r="AQ36" s="36"/>
+    </row>
+    <row r="37" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K37" s="36"/>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
       <c r="X37" s="36"/>
       <c r="AB37" s="36"/>
-      <c r="AF37" s="36"/>
       <c r="AG37" s="36"/>
-      <c r="AP37" s="36"/>
-    </row>
-    <row r="38" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH37" s="36"/>
+      <c r="AQ37" s="36"/>
+    </row>
+    <row r="38" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K38" s="36"/>
       <c r="L38" s="46"/>
       <c r="M38" s="46"/>
       <c r="X38" s="36"/>
       <c r="AB38" s="36"/>
-      <c r="AF38" s="36"/>
       <c r="AG38" s="36"/>
-      <c r="AP38" s="36"/>
-    </row>
-    <row r="39" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH38" s="36"/>
+      <c r="AQ38" s="36"/>
+    </row>
+    <row r="39" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K39" s="36"/>
       <c r="L39" s="46"/>
       <c r="M39" s="46"/>
       <c r="X39" s="36"/>
       <c r="AB39" s="36"/>
-      <c r="AF39" s="36"/>
       <c r="AG39" s="36"/>
-      <c r="AP39" s="36"/>
-    </row>
-    <row r="40" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH39" s="36"/>
+      <c r="AQ39" s="36"/>
+    </row>
+    <row r="40" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K40" s="36"/>
       <c r="L40" s="46"/>
       <c r="M40" s="46"/>
       <c r="X40" s="36"/>
       <c r="AB40" s="36"/>
-      <c r="AF40" s="36"/>
       <c r="AG40" s="36"/>
-      <c r="AP40" s="36"/>
-    </row>
-    <row r="41" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH40" s="36"/>
+      <c r="AQ40" s="36"/>
+    </row>
+    <row r="41" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K41" s="36"/>
       <c r="L41" s="46"/>
       <c r="M41" s="46"/>
       <c r="X41" s="36"/>
       <c r="AB41" s="36"/>
-      <c r="AF41" s="36"/>
       <c r="AG41" s="36"/>
-      <c r="AP41" s="36"/>
-    </row>
-    <row r="42" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH41" s="36"/>
+      <c r="AQ41" s="36"/>
+    </row>
+    <row r="42" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K42" s="36"/>
       <c r="L42" s="46"/>
       <c r="M42" s="46"/>
       <c r="X42" s="36"/>
       <c r="AB42" s="36"/>
-      <c r="AF42" s="36"/>
       <c r="AG42" s="36"/>
-      <c r="AP42" s="36"/>
-    </row>
-    <row r="43" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH42" s="36"/>
+      <c r="AQ42" s="36"/>
+    </row>
+    <row r="43" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K43" s="36"/>
       <c r="L43" s="46"/>
       <c r="M43" s="46"/>
       <c r="X43" s="36"/>
       <c r="AB43" s="36"/>
-      <c r="AF43" s="36"/>
       <c r="AG43" s="36"/>
-      <c r="AP43" s="36"/>
-    </row>
-    <row r="44" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH43" s="36"/>
+      <c r="AQ43" s="36"/>
+    </row>
+    <row r="44" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K44" s="36"/>
       <c r="L44" s="46"/>
       <c r="M44" s="46"/>
       <c r="X44" s="36"/>
       <c r="AB44" s="36"/>
-      <c r="AF44" s="36"/>
       <c r="AG44" s="36"/>
-      <c r="AP44" s="36"/>
-    </row>
-    <row r="45" spans="11:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH44" s="36"/>
+      <c r="AQ44" s="36"/>
+    </row>
+    <row r="45" spans="11:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K45" s="36"/>
       <c r="L45" s="46"/>
       <c r="M45" s="46"/>
       <c r="X45" s="36"/>
       <c r="AB45" s="36"/>
-      <c r="AF45" s="36"/>
       <c r="AG45" s="36"/>
-      <c r="AP45" s="36"/>
+      <c r="AH45" s="36"/>
+      <c r="AQ45" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6774,6 +6786,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6782,61 +6849,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>